<commit_message>
Story 16: Changed Testing Calc
</commit_message>
<xml_diff>
--- a/Homework_3/Portmone_Vlad_Dmytrenko.xlsx
+++ b/Homework_3/Portmone_Vlad_Dmytrenko.xlsx
@@ -722,9 +722,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -739,19 +736,70 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,54 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1130,10 +1130,10 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="21"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1143,10 +1143,10 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="21"/>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -1177,26 +1177,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1204,10 +1204,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="21"/>
     </row>
     <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -1215,10 +1215,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="21"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -1251,10 +1251,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -1279,7 +1279,7 @@
   <dimension ref="B1:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1293,7 @@
       <c r="B1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>100</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1384,7 +1384,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1570,29 +1570,29 @@
       </c>
     </row>
     <row r="31" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>129</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>131</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>120</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -1621,7 +1621,7 @@
       </c>
     </row>
     <row r="36" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>121</v>
       </c>
       <c r="C36" s="9" t="s">
@@ -1668,7 +1668,7 @@
       </c>
     </row>
     <row r="41" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C41" s="9" t="s">
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="45" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="15" t="s">
         <v>123</v>
       </c>
       <c r="C45" s="9" t="s">
@@ -1753,108 +1753,108 @@
       </c>
     </row>
     <row r="50" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="15" t="s">
         <v>133</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B51" s="13"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="13" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B52" s="13"/>
+      <c r="B52" s="12"/>
       <c r="C52" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="13" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B53" s="13"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="13" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B54" s="13"/>
+      <c r="B54" s="12"/>
       <c r="C54" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="13" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B55" s="13"/>
+      <c r="B55" s="12"/>
       <c r="C55" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="13" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B56" s="13"/>
+      <c r="B56" s="12"/>
       <c r="C56" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="13" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B57" s="13"/>
+      <c r="B57" s="12"/>
       <c r="C57" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="13" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B58" s="13"/>
+      <c r="B58" s="12"/>
       <c r="C58" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="13" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B59" s="13"/>
+      <c r="B59" s="12"/>
       <c r="C59" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="13" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B60" s="13"/>
+      <c r="B60" s="12"/>
       <c r="C60" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="13" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="61" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="12" t="s">
         <v>125</v>
       </c>
       <c r="C61" s="9" t="s">
@@ -1928,7 +1928,7 @@
       </c>
     </row>
     <row r="69" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="12" t="s">
         <v>124</v>
       </c>
       <c r="C69" s="9" t="s">
@@ -1993,7 +1993,7 @@
       </c>
     </row>
     <row r="76" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="12" t="s">
         <v>126</v>
       </c>
       <c r="C76" s="9" t="s">
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="87" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="15" t="s">
         <v>128</v>
       </c>
       <c r="C87" s="9" t="s">
@@ -2188,1145 +2188,1141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B48" sqref="B4:C84"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="5" width="29.5703125" customWidth="1"/>
+    <col min="3" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="121.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="23" t="str">
+      <c r="C4" s="28"/>
+      <c r="D4" s="39" t="str">
         <f>'Test scenarios'!B2</f>
         <v>проверка ссылок</v>
       </c>
-      <c r="E4" s="22" t="str">
+      <c r="E4" s="19" t="str">
         <f>'Test scenarios'!C2</f>
         <v>TS_001</v>
       </c>
-      <c r="F4" s="21" t="str">
+      <c r="F4" s="18" t="str">
         <f>'Test scenarios'!D2</f>
         <v>Проверить кликабельность на сайте по переходу на сайты банков-партнеров</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="22" t="str">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="19" t="str">
         <f>'Test scenarios'!C3</f>
         <v>TS_002</v>
       </c>
-      <c r="F5" s="21" t="str">
+      <c r="F5" s="18" t="str">
         <f>'Test scenarios'!D3</f>
         <v>Проверить переход на сайт Google маркет и  App Story</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="22" t="str">
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="19" t="str">
         <f>'Test scenarios'!C4</f>
         <v>TS_003</v>
       </c>
-      <c r="F6" s="21" t="str">
+      <c r="F6" s="18" t="str">
         <f>'Test scenarios'!D4</f>
         <v xml:space="preserve">Проверить корректность перехода из главной страницы на  ссылку "Пополнить счет" </v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="22" t="str">
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="19" t="str">
         <f>'Test scenarios'!C5</f>
         <v>TS_004</v>
       </c>
-      <c r="F7" s="21" t="str">
+      <c r="F7" s="18" t="str">
         <f>'Test scenarios'!D5</f>
         <v>кликаеться сылка "Переводы"</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22" t="str">
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="19" t="str">
         <f>'Test scenarios'!C6</f>
         <v>TS_005</v>
       </c>
-      <c r="F8" s="21" t="str">
+      <c r="F8" s="18" t="str">
         <f>'Test scenarios'!D6</f>
         <v>есть ссылка ведущая на главную страницу</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="22" t="str">
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="19" t="str">
         <f>'Test scenarios'!C7</f>
         <v>TS_006</v>
       </c>
-      <c r="F9" s="21" t="str">
+      <c r="F9" s="18" t="str">
         <f>'Test scenarios'!D7</f>
         <v>есть ли ссылка, которые используються для отправки электронной почты админам сайта</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="22" t="str">
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="19" t="str">
         <f>'Test scenarios'!C8</f>
         <v>TS_007</v>
       </c>
-      <c r="F10" s="21" t="str">
+      <c r="F10" s="18" t="str">
         <f>'Test scenarios'!D8</f>
         <v>Есть ли страницы, на которые не указаны ссылки</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="22" t="str">
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="19" t="str">
         <f>'Test scenarios'!C9</f>
         <v>TS_008</v>
       </c>
-      <c r="F11" s="21" t="str">
+      <c r="F11" s="18" t="str">
         <f>'Test scenarios'!D9</f>
         <v>проверить наличие неработающих ссылок</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22" t="str">
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="19" t="str">
         <f>'Test scenarios'!C10</f>
         <v>TS_009</v>
       </c>
-      <c r="F12" s="21" t="str">
+      <c r="F12" s="18" t="str">
         <f>'Test scenarios'!D10</f>
         <v>Выбрав ссылку "пополнить", "водафон" будет форма для данных, проверить понятно ли для чегопредназначена форма и зачем ее нужно заполнять</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="26" t="str">
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="42" t="str">
         <f>'Test scenarios'!B24</f>
         <v>проверка cookies</v>
       </c>
-      <c r="E13" s="22" t="str">
+      <c r="E13" s="19" t="str">
         <f>'Test scenarios'!C24</f>
         <v>TS_001</v>
       </c>
-      <c r="F13" s="21" t="str">
+      <c r="F13" s="18" t="str">
         <f>'Test scenarios'!D24</f>
         <v>проверить сайт с отключенными cookies</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="22" t="str">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="19" t="str">
         <f>'Test scenarios'!C25</f>
         <v>TS_002</v>
       </c>
-      <c r="F14" s="21" t="str">
+      <c r="F14" s="18" t="str">
         <f>'Test scenarios'!D25</f>
         <v>проверить сайт с включенными cookies</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="22" t="str">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="19" t="str">
         <f>'Test scenarios'!C26</f>
         <v>TS_003</v>
       </c>
-      <c r="F15" s="21" t="str">
+      <c r="F15" s="18" t="str">
         <f>'Test scenarios'!D26</f>
         <v>проверить, что файлы cookies зашифрованы перед записью на компьютер пользователя</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="22" t="str">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="19" t="str">
         <f>'Test scenarios'!C27</f>
         <v>TS_004</v>
       </c>
-      <c r="F16" s="21" t="str">
+      <c r="F16" s="18" t="str">
         <f>'Test scenarios'!D27</f>
         <v>проверить аспекты безопасности при удалении файлов cookies</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="22" t="str">
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="19" t="str">
         <f>'Test scenarios'!C28</f>
         <v>TS_005</v>
       </c>
-      <c r="F17" s="21" t="str">
+      <c r="F17" s="18" t="str">
         <f>'Test scenarios'!D28</f>
         <v>если cookies имеют продолжительность действия, то проверить, активны ли они в указанный период времени</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="26" t="str">
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="42" t="str">
         <f>'Test scenarios'!B29</f>
         <v>HTML/CSS валидация</v>
       </c>
-      <c r="E18" s="22" t="str">
+      <c r="E18" s="19" t="str">
         <f>'Test scenarios'!C29</f>
         <v>TS_001</v>
       </c>
-      <c r="F18" s="21" t="str">
+      <c r="F18" s="18" t="str">
         <f>'Test scenarios'!D29</f>
         <v>проверить код сайта на наличие синтаксических ошибок</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="22" t="str">
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="19" t="str">
         <f>'Test scenarios'!C30</f>
         <v>TS_002</v>
       </c>
-      <c r="F19" s="21" t="str">
+      <c r="F19" s="18" t="str">
         <f>'Test scenarios'!D30</f>
         <v>проверить сайт в том , что он доступен для поисковой системы</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="29" t="str">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="20" t="str">
         <f>'Test scenarios'!B31</f>
         <v>проверка доступности веб-сайта</v>
       </c>
-      <c r="E20" s="22" t="str">
+      <c r="E20" s="19" t="str">
         <f>'Test scenarios'!C31</f>
         <v>TS_001</v>
       </c>
-      <c r="F20" s="21" t="str">
+      <c r="F20" s="18" t="str">
         <f>'Test scenarios'!D31</f>
         <v>проверить, что доступ к сайту с протоколом https имеется по обоим вариантам: и с http, и с https в начале адреса.</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="29" t="str">
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="20" t="str">
         <f>'Test scenarios'!B32</f>
         <v>проверка кроссбраузерность сайта</v>
       </c>
-      <c r="E21" s="22" t="str">
+      <c r="E21" s="19" t="str">
         <f>'Test scenarios'!C32</f>
         <v>TS_001</v>
       </c>
-      <c r="F21" s="21" t="str">
+      <c r="F21" s="18" t="str">
         <f>'Test scenarios'!D32</f>
         <v>зайти на сайт с разных браузеров, и разных версий браузеров</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="30" t="str">
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="22" t="str">
         <f>'Test scenarios'!B61</f>
         <v>проверка совместимости сайта</v>
       </c>
-      <c r="E22" s="22" t="str">
+      <c r="E22" s="19" t="str">
         <f>'Test scenarios'!C61</f>
         <v>TS_001</v>
       </c>
-      <c r="F22" s="21" t="str">
+      <c r="F22" s="18" t="str">
         <f>'Test scenarios'!D61</f>
         <v>проверить конфигурация операционной системы</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="22" t="str">
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="19" t="str">
         <f>'Test scenarios'!C62</f>
         <v>TS_002</v>
       </c>
-      <c r="F23" s="21" t="str">
+      <c r="F23" s="18" t="str">
         <f>'Test scenarios'!D62</f>
         <v>проверить конфигурация браузера</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="22" t="str">
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="19" t="str">
         <f>'Test scenarios'!C63</f>
         <v>TS_003</v>
       </c>
-      <c r="F24" s="21" t="str">
+      <c r="F24" s="18" t="str">
         <f>'Test scenarios'!D63</f>
         <v>проверить конфигурация базы данных</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="22" t="str">
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="19" t="str">
         <f>'Test scenarios'!C64</f>
         <v>TS_004</v>
       </c>
-      <c r="F25" s="21" t="str">
+      <c r="F25" s="18" t="str">
         <f>'Test scenarios'!D64</f>
         <v xml:space="preserve">проверить кросс-платформенность  сайта </v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="22" t="str">
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="19" t="str">
         <f>'Test scenarios'!C65</f>
         <v>TS_005</v>
       </c>
-      <c r="F26" s="21" t="str">
+      <c r="F26" s="18" t="str">
         <f>'Test scenarios'!D65</f>
         <v>проверить кросс-браузерность сайта</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="22" t="str">
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="19" t="str">
         <f>'Test scenarios'!C66</f>
         <v>TS_006</v>
       </c>
-      <c r="F27" s="21" t="str">
+      <c r="F27" s="18" t="str">
         <f>'Test scenarios'!D66</f>
         <v>проверить базу данных</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="22" t="str">
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="19" t="str">
         <f>'Test scenarios'!C67</f>
         <v>TS_007</v>
       </c>
-      <c r="F28" s="21" t="str">
+      <c r="F28" s="18" t="str">
         <f>'Test scenarios'!D67</f>
         <v>Проверить правильность печати шрифтов, графических изображений страниц, выравнивания страниц</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="22" t="str">
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="19" t="str">
         <f>'Test scenarios'!C68</f>
         <v>TS_008</v>
       </c>
-      <c r="F29" s="21" t="str">
+      <c r="F29" s="18" t="str">
         <f>'Test scenarios'!D68</f>
         <v>проверить, что все страницы вашего сайта соответствуют размеру бумаги, определенному в опциях печати</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="35"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="30" t="str">
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="22" t="str">
         <f>'Test scenarios'!B69</f>
         <v>проверка производительности сайта</v>
       </c>
-      <c r="E30" s="22" t="str">
+      <c r="E30" s="19" t="str">
         <f>'Test scenarios'!C69</f>
         <v>TS_001</v>
       </c>
-      <c r="F30" s="21" t="str">
+      <c r="F30" s="18" t="str">
         <f>'Test scenarios'!D69</f>
         <v>проверить поведения сайта на уровне или за пределами его ожидаемой рабочей нагрузки</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="22" t="str">
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="19" t="str">
         <f>'Test scenarios'!C70</f>
         <v>TS_002</v>
       </c>
-      <c r="F31" s="21" t="str">
+      <c r="F31" s="18" t="str">
         <f>'Test scenarios'!D70</f>
         <v xml:space="preserve">проверить поведения сайта при увеличении рабочей нагрузки </v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="35"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="22" t="str">
+      <c r="B32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="19" t="str">
         <f>'Test scenarios'!C71</f>
         <v>TS_003</v>
       </c>
-      <c r="F32" s="21" t="str">
+      <c r="F32" s="18" t="str">
         <f>'Test scenarios'!D71</f>
         <v xml:space="preserve">проверить способности работать в течение или чуть дольше приемлемого периода </v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="35"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="22" t="str">
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="19" t="str">
         <f>'Test scenarios'!C72</f>
         <v>TS_004</v>
       </c>
-      <c r="F33" s="21" t="str">
+      <c r="F33" s="18" t="str">
         <f>'Test scenarios'!D72</f>
         <v xml:space="preserve">проверить производительности веб-сайта за счет увеличения объема данных в базе данных </v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="22" t="str">
+      <c r="B34" s="29"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="19" t="str">
         <f>'Test scenarios'!C73</f>
         <v>TS_005</v>
       </c>
-      <c r="F34" s="21" t="str">
+      <c r="F34" s="18" t="str">
         <f>'Test scenarios'!D73</f>
         <v xml:space="preserve">проверить производительность веб-сайта, при одновременной логинизации большого количества пользователей </v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="22" t="str">
+      <c r="B35" s="29"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="19" t="str">
         <f>'Test scenarios'!C74</f>
         <v>TS_006</v>
       </c>
-      <c r="F35" s="21" t="str">
+      <c r="F35" s="18" t="str">
         <f>'Test scenarios'!D74</f>
         <v xml:space="preserve">проверить поведения сайта при непрерывной дополнительной нагрузке </v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="35"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="22" t="str">
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="19" t="str">
         <f>'Test scenarios'!C75</f>
         <v>TS_007</v>
       </c>
-      <c r="F36" s="21" t="str">
+      <c r="F36" s="18" t="str">
         <f>'Test scenarios'!D75</f>
         <v>проверить скорости загрузки страницы</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="35"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="30" t="str">
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="22" t="str">
         <f>'Test scenarios'!B76</f>
         <v>проверка безопастности функционирования</v>
       </c>
-      <c r="E37" s="22" t="str">
+      <c r="E37" s="19" t="str">
         <f>'Test scenarios'!C76</f>
         <v>TS_001</v>
       </c>
-      <c r="F37" s="21" t="str">
+      <c r="F37" s="18" t="str">
         <f>'Test scenarios'!D76</f>
         <v>если имитировать атаку вредоносного источника</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="22" t="str">
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="19" t="str">
         <f>'Test scenarios'!C77</f>
         <v>TS_002</v>
       </c>
-      <c r="F38" s="21" t="str">
+      <c r="F38" s="18" t="str">
         <f>'Test scenarios'!D77</f>
         <v>проверить уязвимости сайта</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="35"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="22" t="str">
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="19" t="str">
         <f>'Test scenarios'!C78</f>
         <v>TS_003</v>
       </c>
-      <c r="F39" s="21" t="str">
+      <c r="F39" s="18" t="str">
         <f>'Test scenarios'!D78</f>
         <v>если обеспечить невозможность несанкционированного доступа к защищенным страницам</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="35"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="22" t="str">
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="19" t="str">
         <f>'Test scenarios'!C79</f>
         <v>TS_004</v>
       </c>
-      <c r="F40" s="21" t="str">
+      <c r="F40" s="18" t="str">
         <f>'Test scenarios'!D79</f>
         <v>если отключить автоматическое прекращение проверки сеансов  после длительного простоя пользователя</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="35"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="22" t="str">
+      <c r="B41" s="29"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="19" t="str">
         <f>'Test scenarios'!C80</f>
         <v>TS_005</v>
       </c>
-      <c r="F41" s="21" t="str">
+      <c r="F41" s="18" t="str">
         <f>'Test scenarios'!D80</f>
         <v>проверить функций безопасности SSL</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="35"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="22" t="str">
+      <c r="B42" s="29"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="19" t="str">
         <f>'Test scenarios'!C81</f>
         <v>TS_006</v>
       </c>
-      <c r="F42" s="21" t="str">
+      <c r="F42" s="18" t="str">
         <f>'Test scenarios'!D81</f>
         <v xml:space="preserve">Все попытки взлома, сообщения об ошибках, регистрируються и сохраняються в отдельном файле </v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="35"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="22" t="str">
+      <c r="B43" s="29"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="19" t="str">
         <f>'Test scenarios'!C82</f>
         <v>TS_007</v>
       </c>
-      <c r="F43" s="21" t="str">
+      <c r="F43" s="18" t="str">
         <f>'Test scenarios'!D82</f>
         <v>проверить работу captcha с помощью автоматических скриптов</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="22" t="str">
+      <c r="B44" s="29"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="19" t="str">
         <f>'Test scenarios'!C83</f>
         <v>TS_008</v>
       </c>
-      <c r="F44" s="21" t="str">
+      <c r="F44" s="18" t="str">
         <f>'Test scenarios'!D83</f>
         <v>проверить, что файлы с ограниченным доступом не загружаются без соответствующего разрешения</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="35"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="22" t="str">
+      <c r="B45" s="29"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="19" t="str">
         <f>'Test scenarios'!C84</f>
         <v>TS_009</v>
       </c>
-      <c r="F45" s="21" t="str">
+      <c r="F45" s="18" t="str">
         <f>'Test scenarios'!D84</f>
         <v>проверить, что при вводе неправильного пароля или имени пользователя нет возможности входа в систему</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="35"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="30" t="str">
+      <c r="B46" s="29"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="22" t="str">
         <f>'Test scenarios'!B85</f>
         <v>проверка изменений</v>
       </c>
-      <c r="E46" s="22" t="str">
+      <c r="E46" s="19" t="str">
         <f>'Test scenarios'!C85</f>
         <v>TS_001</v>
       </c>
-      <c r="F46" s="21" t="str">
+      <c r="F46" s="18" t="str">
         <f>'Test scenarios'!D85</f>
         <v xml:space="preserve">проверить, что все обнаруженные баги действительно успешно исправлены. </v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="22" t="str">
+      <c r="B47" s="31"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="19" t="str">
         <f>'Test scenarios'!C86</f>
         <v>TS_002</v>
       </c>
-      <c r="F47" s="21" t="str">
+      <c r="F47" s="18" t="str">
         <f>'Test scenarios'!D86</f>
         <v xml:space="preserve">проверить, что не возникли новые баги изменений. </v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="33" t="str">
+      <c r="B48" s="27" t="str">
         <f>FRD!A8</f>
         <v>2. Личный кабинет</v>
       </c>
-      <c r="C48" s="34"/>
-      <c r="D48" s="30" t="str">
+      <c r="C48" s="28"/>
+      <c r="D48" s="22" t="str">
         <f>'Test scenarios'!B33</f>
         <v>навигационная проверка сайта</v>
       </c>
-      <c r="E48" s="22" t="str">
+      <c r="E48" s="19" t="str">
         <f>'Test scenarios'!C33</f>
         <v>TS_001</v>
       </c>
-      <c r="F48" s="21" t="str">
+      <c r="F48" s="18" t="str">
         <f>'Test scenarios'!D33</f>
         <v>Все страницы сайта понятны и просты в использовании.</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="35"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="22" t="str">
+      <c r="B49" s="29"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="19" t="str">
         <f>'Test scenarios'!C34</f>
         <v>TS_002</v>
       </c>
-      <c r="F49" s="21" t="str">
+      <c r="F49" s="18" t="str">
         <f>'Test scenarios'!B24&amp;'Test scenarios'!D24</f>
         <v>проверка cookiesпроверить сайт с отключенными cookies</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="22" t="str">
+      <c r="B50" s="29"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="19" t="str">
         <f>'Test scenarios'!C35</f>
         <v>TS_003</v>
       </c>
-      <c r="F50" s="21" t="str">
+      <c r="F50" s="18" t="str">
         <f>'Test scenarios'!B25&amp;'Test scenarios'!D25</f>
         <v>проверить сайт с включенными cookies</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="35"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="30" t="str">
+      <c r="B51" s="29"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="22" t="str">
         <f>'Test scenarios'!B36</f>
         <v>проверка контента сайта</v>
       </c>
-      <c r="E51" s="22" t="str">
+      <c r="E51" s="19" t="str">
         <f>'Test scenarios'!C36</f>
         <v>TS_001</v>
       </c>
-      <c r="F51" s="21" t="str">
+      <c r="F51" s="18" t="str">
         <f>'Test scenarios'!B26&amp;'Test scenarios'!D26</f>
         <v>проверить, что файлы cookies зашифрованы перед записью на компьютер пользователя</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="35"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="22" t="str">
+      <c r="B52" s="29"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="19" t="str">
         <f>'Test scenarios'!C37</f>
         <v>TS_002</v>
       </c>
-      <c r="F52" s="21" t="str">
+      <c r="F52" s="18" t="str">
         <f>'Test scenarios'!B27&amp;'Test scenarios'!D27</f>
         <v>проверить аспекты безопасности при удалении файлов cookies</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="35"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="22" t="str">
+      <c r="B53" s="29"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="19" t="str">
         <f>'Test scenarios'!C38</f>
         <v>TS_003</v>
       </c>
-      <c r="F53" s="21" t="str">
+      <c r="F53" s="18" t="str">
         <f>'Test scenarios'!B28&amp;'Test scenarios'!D28</f>
         <v>если cookies имеют продолжительность действия, то проверить, активны ли они в указанный период времени</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="35"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="22" t="str">
+      <c r="B54" s="29"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="19" t="str">
         <f>'Test scenarios'!C39</f>
         <v>TS_004</v>
       </c>
-      <c r="F54" s="21" t="str">
+      <c r="F54" s="18" t="str">
         <f>'Test scenarios'!B29&amp;'Test scenarios'!D29</f>
         <v>HTML/CSS валидацияпроверить код сайта на наличие синтаксических ошибок</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="35"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="22" t="str">
+      <c r="B55" s="29"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="19" t="str">
         <f>'Test scenarios'!C40</f>
         <v>TS_005</v>
       </c>
-      <c r="F55" s="21" t="str">
+      <c r="F55" s="18" t="str">
         <f>'Test scenarios'!B30&amp;'Test scenarios'!D30</f>
         <v>проверить сайт в том , что он доступен для поисковой системы</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="35"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="30" t="str">
+      <c r="B56" s="29"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="22" t="str">
         <f>'Test scenarios'!B41</f>
         <v>удобство использования</v>
       </c>
-      <c r="E56" s="22" t="str">
+      <c r="E56" s="19" t="str">
         <f>'Test scenarios'!C41</f>
         <v>TS_001</v>
       </c>
-      <c r="F56" s="21" t="str">
+      <c r="F56" s="18" t="str">
         <f>'Test scenarios'!B31&amp;'Test scenarios'!D31</f>
         <v>проверка доступности веб-сайтапроверить, что доступ к сайту с протоколом https имеется по обоим вариантам: и с http, и с https в начале адреса.</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="35"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="22" t="str">
+      <c r="B57" s="29"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="19" t="str">
         <f>'Test scenarios'!C42</f>
         <v>TS_002</v>
       </c>
-      <c r="F57" s="21" t="str">
+      <c r="F57" s="18" t="str">
         <f>'Test scenarios'!B32&amp;'Test scenarios'!D32</f>
         <v>проверка кроссбраузерность сайтазайти на сайт с разных браузеров, и разных версий браузеров</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="35"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="22" t="str">
+      <c r="B58" s="29"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="19" t="str">
         <f>'Test scenarios'!C43</f>
         <v>TS_003</v>
       </c>
-      <c r="F58" s="21" t="str">
+      <c r="F58" s="18" t="str">
         <f>'Test scenarios'!B33&amp;'Test scenarios'!D33</f>
         <v>навигационная проверка сайтаВсе страницы сайта понятны и просты в использовании.</v>
       </c>
     </row>
     <row r="59" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="35"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="22" t="str">
+      <c r="B59" s="29"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="19" t="str">
         <f>'Test scenarios'!C44</f>
         <v>TS_004</v>
       </c>
-      <c r="F59" s="21" t="str">
+      <c r="F59" s="18" t="str">
         <f>'Test scenarios'!B34&amp;'Test scenarios'!D34</f>
         <v>Кнопки, формы и поля удобны для использования.</v>
       </c>
     </row>
     <row r="60" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="35"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="30" t="str">
+      <c r="B60" s="29"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="22" t="str">
         <f>'Test scenarios'!B45</f>
         <v>проверка использования интерфейса</v>
       </c>
-      <c r="E60" s="22" t="str">
+      <c r="E60" s="19" t="str">
         <f>'Test scenarios'!C45</f>
         <v>TS_001</v>
       </c>
-      <c r="F60" s="21" t="str">
+      <c r="F60" s="18" t="str">
         <f>'Test scenarios'!B35&amp;'Test scenarios'!D35</f>
         <v>Доступ к главному меню осуществляется со всех страниц</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="35"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="22" t="str">
+      <c r="B61" s="29"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="19" t="str">
         <f>'Test scenarios'!C46</f>
         <v>TS_002</v>
       </c>
-      <c r="F61" s="21" t="str">
+      <c r="F61" s="18" t="str">
         <f>'Test scenarios'!B36&amp;'Test scenarios'!D36</f>
         <v>проверка контента сайтаОтсутствуют грамматические, орфографические ошибки</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="35"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="22" t="str">
+      <c r="B62" s="29"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="19" t="str">
         <f>'Test scenarios'!C47</f>
         <v>TS_003</v>
       </c>
-      <c r="F62" s="21" t="str">
+      <c r="F62" s="18" t="str">
         <f>'Test scenarios'!B37&amp;'Test scenarios'!D37</f>
         <v>Изображения имеют соответствующие размеры и размещены правильно</v>
       </c>
     </row>
     <row r="63" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B63" s="35"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="22" t="str">
+      <c r="B63" s="29"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="19" t="str">
         <f>'Test scenarios'!C48</f>
         <v>TS_004</v>
       </c>
-      <c r="F63" s="21" t="str">
+      <c r="F63" s="18" t="str">
         <f>'Test scenarios'!B38&amp;'Test scenarios'!D38</f>
         <v>проверить оптимизацию цветовой палитры сайта и размеры шрифтов</v>
       </c>
     </row>
     <row r="64" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B64" s="35"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="22" t="str">
+      <c r="B64" s="29"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="19" t="str">
         <f>'Test scenarios'!C49</f>
         <v>TS_005</v>
       </c>
-      <c r="F64" s="21" t="str">
+      <c r="F64" s="18" t="str">
         <f>'Test scenarios'!B39&amp;'Test scenarios'!D39</f>
         <v>Контент должен быть информативным, понятным, структурированным и логически связанным</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B65" s="35"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="30" t="str">
+      <c r="B65" s="29"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="22" t="str">
         <f>'Test scenarios'!B50</f>
         <v>проверка мультиязычности сайта</v>
       </c>
-      <c r="E65" s="22" t="str">
+      <c r="E65" s="19" t="str">
         <f>'Test scenarios'!C50</f>
         <v>TS_001</v>
       </c>
-      <c r="F65" s="21" t="str">
+      <c r="F65" s="18" t="str">
         <f>'Test scenarios'!B40&amp;'Test scenarios'!D40</f>
         <v>Инструкции ясны и содержат правильную информацию</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B66" s="35"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="22" t="str">
+      <c r="B66" s="29"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="19" t="str">
         <f>'Test scenarios'!C51</f>
         <v>TS_002</v>
       </c>
-      <c r="F66" s="21" t="str">
+      <c r="F66" s="18" t="str">
         <f>'Test scenarios'!B41&amp;'Test scenarios'!D41</f>
         <v>удобство использованияЯвляется ли сайт понятным и удобным?</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="35"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="22" t="str">
+      <c r="B67" s="29"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="19" t="str">
         <f>'Test scenarios'!C52</f>
         <v>TS_003</v>
       </c>
-      <c r="F67" s="21" t="str">
+      <c r="F67" s="18" t="str">
         <f>'Test scenarios'!B42&amp;'Test scenarios'!D42</f>
         <v>Удобна ли навигация?</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="35"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="22" t="str">
+      <c r="B68" s="29"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="19" t="str">
         <f>'Test scenarios'!C53</f>
         <v>TS_004</v>
       </c>
-      <c r="F68" s="21" t="str">
+      <c r="F68" s="18" t="str">
         <f>'Test scenarios'!B43&amp;'Test scenarios'!D43</f>
         <v>Какое впечатление он производит на пользователя?</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B69" s="35"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="22" t="str">
+      <c r="B69" s="29"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="19" t="str">
         <f>'Test scenarios'!C54</f>
         <v>TS_005</v>
       </c>
-      <c r="F69" s="21" t="str">
+      <c r="F69" s="18" t="str">
         <f>'Test scenarios'!B44&amp;'Test scenarios'!D44</f>
         <v>Есть лишние или ненужные вещи?</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="35"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="22" t="str">
+      <c r="B70" s="29"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="19" t="str">
         <f>'Test scenarios'!C55</f>
         <v>TS_006</v>
       </c>
-      <c r="F70" s="21" t="str">
+      <c r="F70" s="18" t="str">
         <f>'Test scenarios'!B45&amp;'Test scenarios'!D45</f>
         <v>проверка использования интерфейсапроверить оответствие стандартам графических интерфейсов</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B71" s="35"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="22" t="str">
+      <c r="B71" s="29"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="19" t="str">
         <f>'Test scenarios'!C56</f>
         <v>TS_007</v>
       </c>
-      <c r="F71" s="21" t="str">
+      <c r="F71" s="18" t="str">
         <f>'Test scenarios'!B46&amp;'Test scenarios'!D46</f>
         <v>Оценка элементов дизайна: макет, цвета, шрифты, размеры шрифтов, ярлыки, текстовые поля, форматирование текста, титры, кнопки, списки, значки, ссылки</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B72" s="35"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="31"/>
-      <c r="E72" s="22" t="str">
+      <c r="B72" s="29"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="19" t="str">
         <f>'Test scenarios'!C57</f>
         <v>TS_008</v>
       </c>
-      <c r="F72" s="21" t="str">
+      <c r="F72" s="18" t="str">
         <f>'Test scenarios'!B47&amp;'Test scenarios'!D47</f>
         <v>проверить с различными разрешениями экрана</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B73" s="35"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="31"/>
-      <c r="E73" s="22" t="str">
+      <c r="B73" s="29"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="19" t="str">
         <f>'Test scenarios'!C58</f>
         <v>TS_009</v>
       </c>
-      <c r="F73" s="21" t="str">
+      <c r="F73" s="18" t="str">
         <f>'Test scenarios'!B48&amp;'Test scenarios'!D48</f>
         <v>проверить точность перевода, проверка длины имен элементов интерфейса.</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B74" s="35"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="22" t="str">
+      <c r="B74" s="29"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="19" t="str">
         <f>'Test scenarios'!C59</f>
         <v>TS_010</v>
       </c>
-      <c r="F74" s="21" t="str">
+      <c r="F74" s="18" t="str">
         <f>'Test scenarios'!B49&amp;'Test scenarios'!D49</f>
         <v>проверить  графический интерфейс пользователя на целевых устройствах: смартфоны и планшеты</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B75" s="37"/>
-      <c r="C75" s="38"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="22" t="str">
+      <c r="B75" s="31"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="19" t="str">
         <f>'Test scenarios'!C60</f>
         <v>TS_011</v>
       </c>
-      <c r="F75" s="21" t="str">
+      <c r="F75" s="18" t="str">
         <f>'Test scenarios'!B50&amp;'Test scenarios'!D50</f>
         <v>проверка мультиязычности сайтапроверить поддерживаются ли различные языки сайт</v>
       </c>
     </row>
     <row r="76" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="39" t="str">
+      <c r="B76" s="33" t="str">
         <f>FRD!A15</f>
         <v>3. Мобильность</v>
       </c>
-      <c r="C76" s="40"/>
-      <c r="D76" s="30" t="str">
+      <c r="C76" s="34"/>
+      <c r="D76" s="22" t="str">
         <f>'Test scenarios'!B87</f>
         <v>проверка мобильной версии сайта</v>
       </c>
-      <c r="E76" s="22" t="str">
+      <c r="E76" s="19" t="str">
         <f>'Test scenarios'!C87</f>
         <v>TS_001</v>
       </c>
-      <c r="F76" s="21" t="str">
+      <c r="F76" s="18" t="str">
         <f>'Test scenarios'!D87</f>
         <v>Проверить совместимость со смартфонами и планшетами</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B77" s="41"/>
-      <c r="C77" s="42"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="22" t="str">
+      <c r="B77" s="35"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="19" t="str">
         <f>'Test scenarios'!C88</f>
         <v>TS_002</v>
       </c>
-      <c r="F77" s="21" t="str">
+      <c r="F77" s="18" t="str">
         <f>'Test scenarios'!D88</f>
         <v>проверить, что навигация по сайту максимально проста</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B78" s="41"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="22" t="str">
+      <c r="B78" s="35"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="19" t="str">
         <f>'Test scenarios'!C89</f>
         <v>TS_003</v>
       </c>
-      <c r="F78" s="21" t="str">
+      <c r="F78" s="18" t="str">
         <f>'Test scenarios'!D89</f>
         <v>проверить время загрузки  сайта</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B79" s="41"/>
-      <c r="C79" s="42"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="22" t="str">
+      <c r="B79" s="35"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="19" t="str">
         <f>'Test scenarios'!C90</f>
         <v>TS_004</v>
       </c>
-      <c r="F79" s="21" t="str">
+      <c r="F79" s="18" t="str">
         <f>'Test scenarios'!D90</f>
         <v>проверить, что кнопки имеют достаточный размер для людей с большим пальцем</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B80" s="41"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="22" t="str">
+      <c r="B80" s="35"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="19" t="str">
         <f>'Test scenarios'!C91</f>
         <v>TS_005</v>
       </c>
-      <c r="F80" s="21" t="str">
+      <c r="F80" s="18" t="str">
         <f>'Test scenarios'!D91</f>
         <v>проверить размер всех изображений</v>
       </c>
     </row>
     <row r="81" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B81" s="41"/>
-      <c r="C81" s="42"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="22" t="str">
+      <c r="B81" s="35"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="19" t="str">
         <f>'Test scenarios'!C92</f>
         <v>TS_006</v>
       </c>
-      <c r="F81" s="21" t="str">
+      <c r="F81" s="18" t="str">
         <f>'Test scenarios'!D92</f>
         <v>проверить Flash и всплывающие окна</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B82" s="41"/>
-      <c r="C82" s="42"/>
-      <c r="D82" s="31"/>
-      <c r="E82" s="22" t="str">
+      <c r="B82" s="35"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="19" t="str">
         <f>'Test scenarios'!C93</f>
         <v>TS_007</v>
       </c>
-      <c r="F82" s="21" t="str">
+      <c r="F82" s="18" t="str">
         <f>'Test scenarios'!D93</f>
         <v>проверить наличие маркеров и коротких предложений</v>
       </c>
     </row>
     <row r="83" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B83" s="41"/>
-      <c r="C83" s="42"/>
-      <c r="D83" s="31"/>
-      <c r="E83" s="22" t="str">
+      <c r="B83" s="35"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="19" t="str">
         <f>'Test scenarios'!C94</f>
         <v>TS_008</v>
       </c>
-      <c r="F83" s="21" t="str">
+      <c r="F83" s="18" t="str">
         <f>'Test scenarios'!D94</f>
         <v>проверить, что номер телефона может быть набран с помощью одного клика</v>
       </c>
     </row>
     <row r="84" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="43"/>
-      <c r="C84" s="44"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="22" t="str">
+      <c r="B84" s="37"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="19" t="str">
         <f>'Test scenarios'!C95</f>
         <v>TS_009</v>
       </c>
-      <c r="F84" s="21" t="str">
+      <c r="F84" s="18" t="str">
         <f>'Test scenarios'!D95</f>
         <v>проверить, что веб-сайт может получить доступ к местоположению через GPS</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D60:D64"/>
-    <mergeCell ref="D65:D75"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B48:C75"/>
-    <mergeCell ref="B4:C47"/>
     <mergeCell ref="B76:C84"/>
     <mergeCell ref="D76:D84"/>
     <mergeCell ref="D30:D36"/>
@@ -3335,6 +3331,11 @@
     <mergeCell ref="D48:D50"/>
     <mergeCell ref="D51:D55"/>
     <mergeCell ref="D56:D59"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="D65:D75"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B48:C75"/>
+    <mergeCell ref="B4:C47"/>
     <mergeCell ref="D4:D12"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="D18:D19"/>

</xml_diff>

<commit_message>
Story 21: deleted screenshots in document Testing web-site Portmone
</commit_message>
<xml_diff>
--- a/Homework_3/Portmone_Vlad_Dmytrenko.xlsx
+++ b/Homework_3/Portmone_Vlad_Dmytrenko.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7215" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7215" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FRD" sheetId="2" r:id="rId1"/>
@@ -17,14 +17,13 @@
     <sheet name="TM" sheetId="4" r:id="rId3"/>
     <sheet name="tables" sheetId="6" r:id="rId4"/>
     <sheet name="test data" sheetId="8" r:id="rId5"/>
-    <sheet name="picture" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="635">
   <si>
     <t xml:space="preserve">Functional Specification Document: </t>
   </si>
@@ -1930,78 +1929,6 @@
   </si>
   <si>
     <t>проверить правильность перевода полей, кнопок и страниц раздела "нижний колонтитул" и адаптацию его смысл к конкретному языку и национальности,рис.8</t>
-  </si>
-  <si>
-    <t>Рис.1 Меню сайта на русском языке</t>
-  </si>
-  <si>
-    <t>Рис.1 Меню сайта на украинском языке</t>
-  </si>
-  <si>
-    <t>Рис.1 Меню сайта на английском языке</t>
-  </si>
-  <si>
-    <t>Рис.2 Форма регистрации на русском языке</t>
-  </si>
-  <si>
-    <t>Рис.2 Форма регистрации на украинском языке</t>
-  </si>
-  <si>
-    <t>Рис.2 Форма регистрации на английском языке</t>
-  </si>
-  <si>
-    <t>Рис.3 Боковая панель на русском языке</t>
-  </si>
-  <si>
-    <t>Рис.3 Боковая панель на украинском языке</t>
-  </si>
-  <si>
-    <t>Рис.3 Боковая панель на английском языке</t>
-  </si>
-  <si>
-    <t>Рис.5 Раздел "Переводы" на русском языке</t>
-  </si>
-  <si>
-    <t>Рис.4 Раздел "Пополнить счет мобильного телефона" на английском языке</t>
-  </si>
-  <si>
-    <t>Рис.4 Раздел "Пополнить счет мобильного телефона" на украинском языке</t>
-  </si>
-  <si>
-    <t>Рис.4 Раздел "Пополнить счет мобильного телефона" на русском языке</t>
-  </si>
-  <si>
-    <t>Рис.5 Раздел "Переводы" на украинском  языке</t>
-  </si>
-  <si>
-    <t>Рис.5 Раздел "Переводы" на английском  языке</t>
-  </si>
-  <si>
-    <t>Рис.6 Раздел "каталог услуг" на русском  языке</t>
-  </si>
-  <si>
-    <t>Рис.6 Раздел "каталог услуг" на украинском  языке</t>
-  </si>
-  <si>
-    <t>Рис.6 Раздел "каталог услуг" на английском  языке</t>
-  </si>
-  <si>
-    <t>Рис.7 Раздел "оплата по реквизитам" на русском  языке</t>
-  </si>
-  <si>
-    <t>Рис.7 Раздел "оплата по реквизитам" на украинском  языке</t>
-  </si>
-  <si>
-    <t>Рис.7 Раздел "оплата по реквизитам" на английском  языке</t>
-  </si>
-  <si>
-    <t>Рис.8 Раздел "нижний колонтитул" на русском  языке</t>
-  </si>
-  <si>
-    <t>Рис.8 Раздел "нижний колонтитул" на украинском  языке</t>
-  </si>
-  <si>
-    <t>Рис.8 Раздел "нижний колонтитул" на английском  языке</t>
   </si>
 </sst>
 </file>
@@ -2391,7 +2318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2543,42 +2470,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2597,6 +2488,54 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2605,18 +2544,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2627,17 +2554,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2654,1067 +2578,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>3478</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="190500"/>
-          <a:ext cx="10058400" cy="574978"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>12246</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="1143000"/>
-          <a:ext cx="10058400" cy="583746"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>29449</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2095500"/>
-          <a:ext cx="10058400" cy="600949"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>124353</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>181825</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3238500"/>
-          <a:ext cx="3781953" cy="6087325"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>143405</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>181825</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Рисунок 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4267200" y="3238500"/>
-          <a:ext cx="3801005" cy="6087325"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>124353</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>10377</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9144000" y="3238500"/>
-          <a:ext cx="3781953" cy="6106377"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>447993</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>124534</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="9715500"/>
-          <a:ext cx="2276793" cy="5077534"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>505151</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>162639</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Рисунок 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4267200" y="9715500"/>
-          <a:ext cx="2333951" cy="5115639"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>409887</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>10244</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Рисунок 9"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8534400" y="9715500"/>
-          <a:ext cx="2238687" cy="5153744"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>48568</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>67296</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Рисунок 10"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="15420975"/>
-          <a:ext cx="6754168" cy="4448796"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>10462</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>86349</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Рисунок 11"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="20364450"/>
-          <a:ext cx="6716062" cy="4467849"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581957</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>124454</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Рисунок 12"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="25326975"/>
-          <a:ext cx="6677957" cy="4505954"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>334443</xdr:colOff>
-      <xdr:row>178</xdr:row>
-      <xdr:rowOff>105401</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Рисунок 13"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="30089475"/>
-          <a:ext cx="7649643" cy="4486901"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>180</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>220127</xdr:colOff>
-      <xdr:row>203</xdr:row>
-      <xdr:rowOff>86349</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Рисунок 14"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="34851975"/>
-          <a:ext cx="7535327" cy="4467849"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>205</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>220127</xdr:colOff>
-      <xdr:row>228</xdr:row>
-      <xdr:rowOff>143506</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Рисунок 15"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="39614475"/>
-          <a:ext cx="7535327" cy="4525006"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>230</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>429280</xdr:colOff>
-      <xdr:row>247</xdr:row>
-      <xdr:rowOff>162400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Рисунок 16"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="44376975"/>
-          <a:ext cx="4696480" cy="3400900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>249</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>543596</xdr:colOff>
-      <xdr:row>267</xdr:row>
-      <xdr:rowOff>105268</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Рисунок 17"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="47996475"/>
-          <a:ext cx="4810796" cy="3534268"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>269</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>467386</xdr:colOff>
-      <xdr:row>287</xdr:row>
-      <xdr:rowOff>10005</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Рисунок 18"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="51806475"/>
-          <a:ext cx="4734586" cy="3439005"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>289</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>562734</xdr:colOff>
-      <xdr:row>313</xdr:row>
-      <xdr:rowOff>162586</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Рисунок 20"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="55616475"/>
-          <a:ext cx="5439534" cy="4734586"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>315</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>562734</xdr:colOff>
-      <xdr:row>340</xdr:row>
-      <xdr:rowOff>29244</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Рисунок 21"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="60569475"/>
-          <a:ext cx="5439534" cy="4791744"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>342</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>543681</xdr:colOff>
-      <xdr:row>367</xdr:row>
-      <xdr:rowOff>10191</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Рисунок 22"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="65712975"/>
-          <a:ext cx="5420481" cy="4772691"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>369</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>182362</xdr:colOff>
-      <xdr:row>371</xdr:row>
-      <xdr:rowOff>28632</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Рисунок 23"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="70856475"/>
-          <a:ext cx="9935962" cy="409632"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>373</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>201414</xdr:colOff>
-      <xdr:row>375</xdr:row>
-      <xdr:rowOff>28632</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Рисунок 24"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="71618475"/>
-          <a:ext cx="9955014" cy="409632"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>377</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>125204</xdr:colOff>
-      <xdr:row>379</xdr:row>
-      <xdr:rowOff>66737</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Рисунок 25"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="72380475"/>
-          <a:ext cx="9878804" cy="447737"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4131,8 +2994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D216"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6170,11 +5033,11 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="64" t="str">
+      <c r="C4" s="71" t="str">
         <f>FRD!A3</f>
         <v>1.Меню-сайта</v>
       </c>
-      <c r="D4" s="59" t="str">
+      <c r="D4" s="74" t="str">
         <f>overview!B2</f>
         <v>1.1 проверить наличие, расположение, графический интерфейс кнопок меню</v>
       </c>
@@ -6189,8 +5052,8 @@
     </row>
     <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="42"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="75"/>
       <c r="E5" s="40" t="str">
         <f>overview!C3</f>
         <v>1.1.2</v>
@@ -6202,8 +5065,8 @@
     </row>
     <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="42"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="60"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="75"/>
       <c r="E6" s="40" t="str">
         <f>overview!C4</f>
         <v>1.1.3</v>
@@ -6215,8 +5078,8 @@
     </row>
     <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="42"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="60"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="40" t="str">
         <f>overview!C5</f>
         <v>1.1.4</v>
@@ -6228,8 +5091,8 @@
     </row>
     <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="42"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="60"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="75"/>
       <c r="E8" s="40" t="str">
         <f>overview!C6</f>
         <v>1.1.5</v>
@@ -6241,8 +5104,8 @@
     </row>
     <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="42"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="60"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="75"/>
       <c r="E9" s="40" t="str">
         <f>overview!C7</f>
         <v>1.1.6</v>
@@ -6254,8 +5117,8 @@
     </row>
     <row r="10" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" s="42"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="60"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="75"/>
       <c r="E10" s="40" t="str">
         <f>overview!C8</f>
         <v>1.1.7</v>
@@ -6267,8 +5130,8 @@
     </row>
     <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="42"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="60" t="str">
+      <c r="C11" s="72"/>
+      <c r="D11" s="75" t="str">
         <f>overview!B9</f>
         <v>1.2 Проверить кликабельность, соответствие и коректность кнопок меню</v>
       </c>
@@ -6283,8 +5146,8 @@
     </row>
     <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="42"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="60"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="75"/>
       <c r="E12" s="40" t="str">
         <f>overview!C10</f>
         <v>1.2.2</v>
@@ -6296,8 +5159,8 @@
     </row>
     <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="60"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="75"/>
       <c r="E13" s="40" t="str">
         <f>overview!C11</f>
         <v>1.2.3</v>
@@ -6309,8 +5172,8 @@
     </row>
     <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="60"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="75"/>
       <c r="E14" s="40" t="str">
         <f>overview!C12</f>
         <v>1.2.4</v>
@@ -6322,8 +5185,8 @@
     </row>
     <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="60"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="75"/>
       <c r="E15" s="40" t="str">
         <f>overview!C13</f>
         <v>1.2.5</v>
@@ -6335,8 +5198,8 @@
     </row>
     <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="60"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="40" t="str">
         <f>overview!C14</f>
         <v>1.2.6</v>
@@ -6348,8 +5211,8 @@
     </row>
     <row r="17" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="60"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="75"/>
       <c r="E17" s="40" t="str">
         <f>overview!C15</f>
         <v>1.2.7</v>
@@ -6361,8 +5224,8 @@
     </row>
     <row r="18" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="60"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="40" t="str">
         <f>overview!C16</f>
         <v>1.2.8</v>
@@ -6374,8 +5237,8 @@
     </row>
     <row r="19" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="42"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="61"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="76"/>
       <c r="E19" s="51" t="str">
         <f>overview!C17</f>
         <v>1.2.9</v>
@@ -6387,11 +5250,11 @@
     </row>
     <row r="20" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
-      <c r="C20" s="64" t="str">
+      <c r="C20" s="71" t="str">
         <f>FRD!A5</f>
         <v>2."Войти"</v>
       </c>
-      <c r="D20" s="62" t="str">
+      <c r="D20" s="68" t="str">
         <f>overview!B18</f>
         <v>2.1 Проверить кликабельность, соответствие и корректность использование кнопки "Войти"</v>
       </c>
@@ -6406,8 +5269,8 @@
     </row>
     <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="42"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="63"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="69"/>
       <c r="E21" s="40" t="str">
         <f>overview!C19</f>
         <v>2.1.2</v>
@@ -6419,8 +5282,8 @@
     </row>
     <row r="22" spans="2:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="69"/>
       <c r="E22" s="40" t="str">
         <f>overview!C20</f>
         <v>2.1.3</v>
@@ -6432,8 +5295,8 @@
     </row>
     <row r="23" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="42"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="63" t="str">
+      <c r="C23" s="72"/>
+      <c r="D23" s="69" t="str">
         <f>overview!B21</f>
         <v>2.2 Проверить ввода данных форму</v>
       </c>
@@ -6448,8 +5311,8 @@
     </row>
     <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="42"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="63"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="69"/>
       <c r="E24" s="40" t="str">
         <f>overview!C22</f>
         <v>2.2.2</v>
@@ -6461,8 +5324,8 @@
     </row>
     <row r="25" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="42"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="63"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="69"/>
       <c r="E25" s="40" t="str">
         <f>overview!C23</f>
         <v>2.2.3</v>
@@ -6474,8 +5337,8 @@
     </row>
     <row r="26" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="42"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="63"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="69"/>
       <c r="E26" s="40" t="str">
         <f>overview!C24</f>
         <v>2.2.4</v>
@@ -6487,8 +5350,8 @@
     </row>
     <row r="27" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="42"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="63"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="69"/>
       <c r="E27" s="40" t="str">
         <f>overview!C25</f>
         <v>2.2.5</v>
@@ -6500,8 +5363,8 @@
     </row>
     <row r="28" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="42"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="63"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="69"/>
       <c r="E28" s="40" t="str">
         <f>overview!C26</f>
         <v>2.2.6</v>
@@ -6513,8 +5376,8 @@
     </row>
     <row r="29" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="42"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="63"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="69"/>
       <c r="E29" s="40" t="str">
         <f>overview!C27</f>
         <v>2.2.7</v>
@@ -6526,8 +5389,8 @@
     </row>
     <row r="30" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="42"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="63"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="69"/>
       <c r="E30" s="40" t="str">
         <f>overview!C28</f>
         <v>2.2.8</v>
@@ -6539,8 +5402,8 @@
     </row>
     <row r="31" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="42"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="63"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="69"/>
       <c r="E31" s="40" t="str">
         <f>overview!C29</f>
         <v>2.2.9</v>
@@ -6552,8 +5415,8 @@
     </row>
     <row r="32" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="42"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="63"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="69"/>
       <c r="E32" s="40" t="str">
         <f>overview!C30</f>
         <v>2.2.10</v>
@@ -6565,8 +5428,8 @@
     </row>
     <row r="33" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="42"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="63"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="69"/>
       <c r="E33" s="40" t="str">
         <f>overview!C31</f>
         <v>2.2.11</v>
@@ -6578,8 +5441,8 @@
     </row>
     <row r="34" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="42"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="63"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="69"/>
       <c r="E34" s="40" t="str">
         <f>overview!C32</f>
         <v>2.2.12</v>
@@ -6591,8 +5454,8 @@
     </row>
     <row r="35" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="42"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="63"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="69"/>
       <c r="E35" s="40" t="str">
         <f>overview!C33</f>
         <v>2.2.13</v>
@@ -6604,8 +5467,8 @@
     </row>
     <row r="36" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="42"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="63"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="69"/>
       <c r="E36" s="40" t="str">
         <f>overview!C34</f>
         <v>2.2.14</v>
@@ -6617,8 +5480,8 @@
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="42"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="63"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="69"/>
       <c r="E37" s="40" t="str">
         <f>overview!C35</f>
         <v>2.2.15</v>
@@ -6630,8 +5493,8 @@
     </row>
     <row r="38" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="42"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="63"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="69"/>
       <c r="E38" s="40" t="str">
         <f>overview!C36</f>
         <v>2.2.16</v>
@@ -6643,8 +5506,8 @@
     </row>
     <row r="39" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="42"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="63"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="69"/>
       <c r="E39" s="40" t="str">
         <f>overview!C37</f>
         <v>2.2.17</v>
@@ -6656,8 +5519,8 @@
     </row>
     <row r="40" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="42"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="63"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="69"/>
       <c r="E40" s="40" t="str">
         <f>overview!C38</f>
         <v>2.2.18</v>
@@ -6669,8 +5532,8 @@
     </row>
     <row r="41" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="42"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="63"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="69"/>
       <c r="E41" s="40" t="str">
         <f>overview!C39</f>
         <v>2.2.19</v>
@@ -6682,8 +5545,8 @@
     </row>
     <row r="42" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B42" s="42"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="63"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="69"/>
       <c r="E42" s="40" t="str">
         <f>overview!C40</f>
         <v>2.2.20</v>
@@ -6695,8 +5558,8 @@
     </row>
     <row r="43" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="42"/>
-      <c r="C43" s="66"/>
-      <c r="D43" s="67"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="51" t="str">
         <f>overview!C41</f>
         <v>2.2.21</v>
@@ -6708,11 +5571,11 @@
     </row>
     <row r="44" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="42"/>
-      <c r="C44" s="64" t="str">
+      <c r="C44" s="71" t="str">
         <f>FRD!A7</f>
         <v>3. "Зарегестрироваться"</v>
       </c>
-      <c r="D44" s="62" t="str">
+      <c r="D44" s="68" t="str">
         <f>overview!B42</f>
         <v>3.1 Проверить кликабельность, соответствие и корректность использование кнопки "Зарегистрироваться"</v>
       </c>
@@ -6727,8 +5590,8 @@
     </row>
     <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="42"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="63"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="69"/>
       <c r="E45" s="40" t="str">
         <f>overview!C43</f>
         <v>3.1.2</v>
@@ -6740,8 +5603,8 @@
     </row>
     <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="42"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="63"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="40" t="str">
         <f>overview!C44</f>
         <v>3.1.3</v>
@@ -6753,8 +5616,8 @@
     </row>
     <row r="47" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="43"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="63" t="str">
+      <c r="C47" s="72"/>
+      <c r="D47" s="69" t="str">
         <f>overview!B45</f>
         <v>3.2 Проверить ввода данных форму регистрации</v>
       </c>
@@ -6769,8 +5632,8 @@
     </row>
     <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="41"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="63"/>
+      <c r="C48" s="72"/>
+      <c r="D48" s="69"/>
       <c r="E48" s="40" t="str">
         <f>overview!C46</f>
         <v>3.2.4</v>
@@ -6782,8 +5645,8 @@
     </row>
     <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="42"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="63"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="69"/>
       <c r="E49" s="40" t="str">
         <f>overview!C47</f>
         <v>3.2.5</v>
@@ -6795,8 +5658,8 @@
     </row>
     <row r="50" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="42"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="63"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="69"/>
       <c r="E50" s="40" t="str">
         <f>overview!C48</f>
         <v>3.2.6</v>
@@ -6808,8 +5671,8 @@
     </row>
     <row r="51" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="42"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="63"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="69"/>
       <c r="E51" s="40" t="str">
         <f>overview!C49</f>
         <v>3.2.7</v>
@@ -6821,8 +5684,8 @@
     </row>
     <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="42"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="63"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="69"/>
       <c r="E52" s="40" t="str">
         <f>overview!C50</f>
         <v>3.2.8</v>
@@ -6834,8 +5697,8 @@
     </row>
     <row r="53" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="42"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="63"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="69"/>
       <c r="E53" s="40" t="str">
         <f>overview!C51</f>
         <v>3.2.9</v>
@@ -6847,8 +5710,8 @@
     </row>
     <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="42"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="63"/>
+      <c r="C54" s="72"/>
+      <c r="D54" s="69"/>
       <c r="E54" s="40" t="str">
         <f>overview!C52</f>
         <v>3.2.10</v>
@@ -6860,8 +5723,8 @@
     </row>
     <row r="55" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="42"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="63"/>
+      <c r="C55" s="72"/>
+      <c r="D55" s="69"/>
       <c r="E55" s="40" t="str">
         <f>overview!C53</f>
         <v>3.2.11</v>
@@ -6873,8 +5736,8 @@
     </row>
     <row r="56" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="42"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="63"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="69"/>
       <c r="E56" s="40" t="str">
         <f>overview!C54</f>
         <v>3.2.12</v>
@@ -6886,8 +5749,8 @@
     </row>
     <row r="57" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="42"/>
-      <c r="C57" s="65"/>
-      <c r="D57" s="63"/>
+      <c r="C57" s="72"/>
+      <c r="D57" s="69"/>
       <c r="E57" s="40" t="str">
         <f>overview!C55</f>
         <v>3.2.13</v>
@@ -6899,8 +5762,8 @@
     </row>
     <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="42"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="63"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="69"/>
       <c r="E58" s="40" t="str">
         <f>overview!C56</f>
         <v>3.2.14</v>
@@ -6912,8 +5775,8 @@
     </row>
     <row r="59" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="42"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="63"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="69"/>
       <c r="E59" s="40" t="str">
         <f>overview!C57</f>
         <v>3.2.15</v>
@@ -6925,8 +5788,8 @@
     </row>
     <row r="60" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="42"/>
-      <c r="C60" s="65"/>
-      <c r="D60" s="63"/>
+      <c r="C60" s="72"/>
+      <c r="D60" s="69"/>
       <c r="E60" s="40" t="str">
         <f>overview!C58</f>
         <v>3.2.16</v>
@@ -6938,8 +5801,8 @@
     </row>
     <row r="61" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="42"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="63"/>
+      <c r="C61" s="72"/>
+      <c r="D61" s="69"/>
       <c r="E61" s="40" t="str">
         <f>overview!C59</f>
         <v>3.2.17</v>
@@ -6951,8 +5814,8 @@
     </row>
     <row r="62" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="42"/>
-      <c r="C62" s="65"/>
-      <c r="D62" s="63"/>
+      <c r="C62" s="72"/>
+      <c r="D62" s="69"/>
       <c r="E62" s="40" t="str">
         <f>overview!C60</f>
         <v>3.2.18</v>
@@ -6964,8 +5827,8 @@
     </row>
     <row r="63" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="42"/>
-      <c r="C63" s="65"/>
-      <c r="D63" s="63"/>
+      <c r="C63" s="72"/>
+      <c r="D63" s="69"/>
       <c r="E63" s="40" t="str">
         <f>overview!C61</f>
         <v>3.2.19</v>
@@ -6977,8 +5840,8 @@
     </row>
     <row r="64" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="42"/>
-      <c r="C64" s="65"/>
-      <c r="D64" s="63"/>
+      <c r="C64" s="72"/>
+      <c r="D64" s="69"/>
       <c r="E64" s="40" t="str">
         <f>overview!C62</f>
         <v>3.2.20</v>
@@ -6990,8 +5853,8 @@
     </row>
     <row r="65" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="42"/>
-      <c r="C65" s="65"/>
-      <c r="D65" s="63"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="69"/>
       <c r="E65" s="40" t="str">
         <f>overview!C63</f>
         <v>3.2.21</v>
@@ -7003,8 +5866,8 @@
     </row>
     <row r="66" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="42"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="63"/>
+      <c r="C66" s="72"/>
+      <c r="D66" s="69"/>
       <c r="E66" s="40" t="str">
         <f>overview!C64</f>
         <v>3.2.22</v>
@@ -7016,8 +5879,8 @@
     </row>
     <row r="67" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="42"/>
-      <c r="C67" s="65"/>
-      <c r="D67" s="63"/>
+      <c r="C67" s="72"/>
+      <c r="D67" s="69"/>
       <c r="E67" s="40" t="str">
         <f>overview!C65</f>
         <v>3.2.23</v>
@@ -7029,8 +5892,8 @@
     </row>
     <row r="68" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="42"/>
-      <c r="C68" s="65"/>
-      <c r="D68" s="63"/>
+      <c r="C68" s="72"/>
+      <c r="D68" s="69"/>
       <c r="E68" s="40" t="str">
         <f>overview!C66</f>
         <v>3.2.24</v>
@@ -7042,8 +5905,8 @@
     </row>
     <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="42"/>
-      <c r="C69" s="65"/>
-      <c r="D69" s="63"/>
+      <c r="C69" s="72"/>
+      <c r="D69" s="69"/>
       <c r="E69" s="40" t="str">
         <f>overview!C67</f>
         <v>3.2.25</v>
@@ -7055,8 +5918,8 @@
     </row>
     <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="42"/>
-      <c r="C70" s="65"/>
-      <c r="D70" s="63"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="69"/>
       <c r="E70" s="40" t="str">
         <f>overview!C68</f>
         <v>3.2.26</v>
@@ -7068,8 +5931,8 @@
     </row>
     <row r="71" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="42"/>
-      <c r="C71" s="65"/>
-      <c r="D71" s="63"/>
+      <c r="C71" s="72"/>
+      <c r="D71" s="69"/>
       <c r="E71" s="40" t="str">
         <f>overview!C69</f>
         <v>3.2.27</v>
@@ -7081,8 +5944,8 @@
     </row>
     <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="42"/>
-      <c r="C72" s="65"/>
-      <c r="D72" s="63"/>
+      <c r="C72" s="72"/>
+      <c r="D72" s="69"/>
       <c r="E72" s="40" t="str">
         <f>overview!C70</f>
         <v>3.2.28</v>
@@ -7094,8 +5957,8 @@
     </row>
     <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="42"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="63"/>
+      <c r="C73" s="72"/>
+      <c r="D73" s="69"/>
       <c r="E73" s="40" t="str">
         <f>overview!C71</f>
         <v>3.2.29</v>
@@ -7107,8 +5970,8 @@
     </row>
     <row r="74" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="42"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="63"/>
+      <c r="C74" s="72"/>
+      <c r="D74" s="69"/>
       <c r="E74" s="40" t="str">
         <f>overview!C72</f>
         <v>3.2.30</v>
@@ -7120,8 +5983,8 @@
     </row>
     <row r="75" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="43"/>
-      <c r="C75" s="65"/>
-      <c r="D75" s="63"/>
+      <c r="C75" s="72"/>
+      <c r="D75" s="69"/>
       <c r="E75" s="40" t="str">
         <f>overview!C73</f>
         <v>3.2.31</v>
@@ -7133,8 +5996,8 @@
     </row>
     <row r="76" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B76" s="44"/>
-      <c r="C76" s="65"/>
-      <c r="D76" s="63"/>
+      <c r="C76" s="72"/>
+      <c r="D76" s="69"/>
       <c r="E76" s="40" t="str">
         <f>overview!C74</f>
         <v>3.2.32</v>
@@ -7146,8 +6009,8 @@
     </row>
     <row r="77" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B77" s="45"/>
-      <c r="C77" s="65"/>
-      <c r="D77" s="63"/>
+      <c r="C77" s="72"/>
+      <c r="D77" s="69"/>
       <c r="E77" s="40" t="str">
         <f>overview!C75</f>
         <v>3.2.33</v>
@@ -7159,8 +6022,8 @@
     </row>
     <row r="78" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="45"/>
-      <c r="C78" s="65"/>
-      <c r="D78" s="63" t="str">
+      <c r="C78" s="72"/>
+      <c r="D78" s="69" t="str">
         <f>overview!B76</f>
         <v>3.3 проверить наличие, расположение, графический интерфейс кнопки "Зарегистрироваться"</v>
       </c>
@@ -7175,8 +6038,8 @@
     </row>
     <row r="79" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="45"/>
-      <c r="C79" s="65"/>
-      <c r="D79" s="63"/>
+      <c r="C79" s="72"/>
+      <c r="D79" s="69"/>
       <c r="E79" s="40" t="str">
         <f>overview!C77</f>
         <v>3.3.2</v>
@@ -7188,8 +6051,8 @@
     </row>
     <row r="80" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B80" s="45"/>
-      <c r="C80" s="65"/>
-      <c r="D80" s="63"/>
+      <c r="C80" s="72"/>
+      <c r="D80" s="69"/>
       <c r="E80" s="40" t="str">
         <f>overview!C78</f>
         <v>3.3.3</v>
@@ -7201,8 +6064,8 @@
     </row>
     <row r="81" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="45"/>
-      <c r="C81" s="65"/>
-      <c r="D81" s="63"/>
+      <c r="C81" s="72"/>
+      <c r="D81" s="69"/>
       <c r="E81" s="40" t="str">
         <f>overview!C79</f>
         <v>3.3.4</v>
@@ -7214,8 +6077,8 @@
     </row>
     <row r="82" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="45"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="63"/>
+      <c r="C82" s="72"/>
+      <c r="D82" s="69"/>
       <c r="E82" s="40" t="str">
         <f>overview!C80</f>
         <v>3.3.5</v>
@@ -7227,8 +6090,8 @@
     </row>
     <row r="83" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="45"/>
-      <c r="C83" s="65"/>
-      <c r="D83" s="63"/>
+      <c r="C83" s="72"/>
+      <c r="D83" s="69"/>
       <c r="E83" s="40" t="str">
         <f>overview!C81</f>
         <v>3.3.6</v>
@@ -7240,8 +6103,8 @@
     </row>
     <row r="84" spans="2:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="46"/>
-      <c r="C84" s="66"/>
-      <c r="D84" s="67"/>
+      <c r="C84" s="73"/>
+      <c r="D84" s="70"/>
       <c r="E84" s="51" t="str">
         <f>overview!C82</f>
         <v>3.3.7</v>
@@ -7252,11 +6115,11 @@
       </c>
     </row>
     <row r="85" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C85" s="74" t="str">
+      <c r="C85" s="62" t="str">
         <f>FRD!A10</f>
         <v>4. Боковая панель</v>
       </c>
-      <c r="D85" s="68" t="str">
+      <c r="D85" s="65" t="str">
         <f>overview!B83</f>
         <v>4.1 проверить наличие, расположение, графический интерфейс боковой панели</v>
       </c>
@@ -7270,8 +6133,8 @@
       </c>
     </row>
     <row r="86" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C86" s="75"/>
-      <c r="D86" s="69"/>
+      <c r="C86" s="63"/>
+      <c r="D86" s="66"/>
       <c r="E86" s="40" t="str">
         <f>overview!C84</f>
         <v>4.1.2</v>
@@ -7282,8 +6145,8 @@
       </c>
     </row>
     <row r="87" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C87" s="75"/>
-      <c r="D87" s="69"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="66"/>
       <c r="E87" s="40" t="str">
         <f>overview!C85</f>
         <v>4.1.3</v>
@@ -7294,8 +6157,8 @@
       </c>
     </row>
     <row r="88" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C88" s="75"/>
-      <c r="D88" s="69"/>
+      <c r="C88" s="63"/>
+      <c r="D88" s="66"/>
       <c r="E88" s="40" t="str">
         <f>overview!C86</f>
         <v>4.1.4</v>
@@ -7306,8 +6169,8 @@
       </c>
     </row>
     <row r="89" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C89" s="75"/>
-      <c r="D89" s="69"/>
+      <c r="C89" s="63"/>
+      <c r="D89" s="66"/>
       <c r="E89" s="40" t="str">
         <f>overview!C87</f>
         <v>4.1.5</v>
@@ -7318,8 +6181,8 @@
       </c>
     </row>
     <row r="90" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C90" s="75"/>
-      <c r="D90" s="69"/>
+      <c r="C90" s="63"/>
+      <c r="D90" s="66"/>
       <c r="E90" s="40" t="str">
         <f>overview!C88</f>
         <v>4.1.6</v>
@@ -7330,8 +6193,8 @@
       </c>
     </row>
     <row r="91" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C91" s="75"/>
-      <c r="D91" s="69"/>
+      <c r="C91" s="63"/>
+      <c r="D91" s="66"/>
       <c r="E91" s="40" t="str">
         <f>overview!C89</f>
         <v>4.1.7</v>
@@ -7342,8 +6205,8 @@
       </c>
     </row>
     <row r="92" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C92" s="75"/>
-      <c r="D92" s="69"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="66"/>
       <c r="E92" s="40" t="str">
         <f>overview!C90</f>
         <v>4.1.8</v>
@@ -7354,8 +6217,8 @@
       </c>
     </row>
     <row r="93" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C93" s="75"/>
-      <c r="D93" s="69" t="str">
+      <c r="C93" s="63"/>
+      <c r="D93" s="66" t="str">
         <f>overview!B91</f>
         <v>4.2 Проверить кликабельность, соответствие и коректность боковой панели</v>
       </c>
@@ -7369,8 +6232,8 @@
       </c>
     </row>
     <row r="94" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C94" s="75"/>
-      <c r="D94" s="69"/>
+      <c r="C94" s="63"/>
+      <c r="D94" s="66"/>
       <c r="E94" s="40" t="str">
         <f>overview!C92</f>
         <v>4.2.2</v>
@@ -7381,8 +6244,8 @@
       </c>
     </row>
     <row r="95" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C95" s="75"/>
-      <c r="D95" s="69"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="66"/>
       <c r="E95" s="40" t="str">
         <f>overview!C93</f>
         <v>4.2.3</v>
@@ -7393,8 +6256,8 @@
       </c>
     </row>
     <row r="96" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C96" s="75"/>
-      <c r="D96" s="69"/>
+      <c r="C96" s="63"/>
+      <c r="D96" s="66"/>
       <c r="E96" s="40" t="str">
         <f>overview!C94</f>
         <v>4.2.4</v>
@@ -7405,8 +6268,8 @@
       </c>
     </row>
     <row r="97" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C97" s="75"/>
-      <c r="D97" s="69"/>
+      <c r="C97" s="63"/>
+      <c r="D97" s="66"/>
       <c r="E97" s="40" t="str">
         <f>overview!C95</f>
         <v>4.2.5</v>
@@ -7417,8 +6280,8 @@
       </c>
     </row>
     <row r="98" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C98" s="75"/>
-      <c r="D98" s="69"/>
+      <c r="C98" s="63"/>
+      <c r="D98" s="66"/>
       <c r="E98" s="40" t="str">
         <f>overview!C96</f>
         <v>4.2.6</v>
@@ -7429,8 +6292,8 @@
       </c>
     </row>
     <row r="99" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C99" s="75"/>
-      <c r="D99" s="69"/>
+      <c r="C99" s="63"/>
+      <c r="D99" s="66"/>
       <c r="E99" s="40" t="str">
         <f>overview!C97</f>
         <v>4.2.7</v>
@@ -7441,8 +6304,8 @@
       </c>
     </row>
     <row r="100" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C100" s="76"/>
-      <c r="D100" s="70"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="67"/>
       <c r="E100" s="51" t="str">
         <f>overview!C98</f>
         <v>4.2.8</v>
@@ -7453,11 +6316,11 @@
       </c>
     </row>
     <row r="101" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C101" s="71" t="str">
+      <c r="C101" s="59" t="str">
         <f>FRD!A12</f>
         <v>5. Раздел "пополнение мобильного телефона"</v>
       </c>
-      <c r="D101" s="68" t="str">
+      <c r="D101" s="65" t="str">
         <f>overview!B99</f>
         <v>5.1 Проверить ввода данных форму пополнение мобильного телефона</v>
       </c>
@@ -7471,8 +6334,8 @@
       </c>
     </row>
     <row r="102" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C102" s="72"/>
-      <c r="D102" s="69"/>
+      <c r="C102" s="60"/>
+      <c r="D102" s="66"/>
       <c r="E102" s="40" t="str">
         <f>overview!C100</f>
         <v>5.1.2</v>
@@ -7483,8 +6346,8 @@
       </c>
     </row>
     <row r="103" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C103" s="72"/>
-      <c r="D103" s="69"/>
+      <c r="C103" s="60"/>
+      <c r="D103" s="66"/>
       <c r="E103" s="40" t="str">
         <f>overview!C101</f>
         <v>5.1.3</v>
@@ -7495,8 +6358,8 @@
       </c>
     </row>
     <row r="104" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C104" s="72"/>
-      <c r="D104" s="69"/>
+      <c r="C104" s="60"/>
+      <c r="D104" s="66"/>
       <c r="E104" s="40" t="str">
         <f>overview!C102</f>
         <v>5.1.4</v>
@@ -7507,8 +6370,8 @@
       </c>
     </row>
     <row r="105" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C105" s="72"/>
-      <c r="D105" s="69"/>
+      <c r="C105" s="60"/>
+      <c r="D105" s="66"/>
       <c r="E105" s="40" t="str">
         <f>overview!C103</f>
         <v>5.1.5</v>
@@ -7519,8 +6382,8 @@
       </c>
     </row>
     <row r="106" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C106" s="72"/>
-      <c r="D106" s="69"/>
+      <c r="C106" s="60"/>
+      <c r="D106" s="66"/>
       <c r="E106" s="40" t="str">
         <f>overview!C104</f>
         <v>5.1.6</v>
@@ -7531,8 +6394,8 @@
       </c>
     </row>
     <row r="107" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C107" s="72"/>
-      <c r="D107" s="69"/>
+      <c r="C107" s="60"/>
+      <c r="D107" s="66"/>
       <c r="E107" s="40" t="str">
         <f>overview!C105</f>
         <v>5.1.7</v>
@@ -7543,8 +6406,8 @@
       </c>
     </row>
     <row r="108" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C108" s="72"/>
-      <c r="D108" s="69"/>
+      <c r="C108" s="60"/>
+      <c r="D108" s="66"/>
       <c r="E108" s="40" t="str">
         <f>overview!C106</f>
         <v>5.1.8</v>
@@ -7555,8 +6418,8 @@
       </c>
     </row>
     <row r="109" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C109" s="72"/>
-      <c r="D109" s="69"/>
+      <c r="C109" s="60"/>
+      <c r="D109" s="66"/>
       <c r="E109" s="40" t="str">
         <f>overview!C107</f>
         <v>5.1.9</v>
@@ -7567,8 +6430,8 @@
       </c>
     </row>
     <row r="110" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C110" s="72"/>
-      <c r="D110" s="69" t="str">
+      <c r="C110" s="60"/>
+      <c r="D110" s="66" t="str">
         <f>overview!B108</f>
         <v>5.2 Проверить кликабельность, соответствие и коректность формы "пополнение мобильного телефона"</v>
       </c>
@@ -7582,8 +6445,8 @@
       </c>
     </row>
     <row r="111" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C111" s="72"/>
-      <c r="D111" s="69"/>
+      <c r="C111" s="60"/>
+      <c r="D111" s="66"/>
       <c r="E111" s="40" t="str">
         <f>overview!C109</f>
         <v>5.2.2</v>
@@ -7594,8 +6457,8 @@
       </c>
     </row>
     <row r="112" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C112" s="72"/>
-      <c r="D112" s="69"/>
+      <c r="C112" s="60"/>
+      <c r="D112" s="66"/>
       <c r="E112" s="40" t="str">
         <f>overview!C110</f>
         <v>5.2.3</v>
@@ -7606,8 +6469,8 @@
       </c>
     </row>
     <row r="113" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C113" s="72"/>
-      <c r="D113" s="69"/>
+      <c r="C113" s="60"/>
+      <c r="D113" s="66"/>
       <c r="E113" s="40" t="str">
         <f>overview!C111</f>
         <v>5.2.4</v>
@@ -7618,8 +6481,8 @@
       </c>
     </row>
     <row r="114" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C114" s="72"/>
-      <c r="D114" s="69"/>
+      <c r="C114" s="60"/>
+      <c r="D114" s="66"/>
       <c r="E114" s="40" t="str">
         <f>overview!C112</f>
         <v>5.2.5</v>
@@ -7630,8 +6493,8 @@
       </c>
     </row>
     <row r="115" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C115" s="72"/>
-      <c r="D115" s="69"/>
+      <c r="C115" s="60"/>
+      <c r="D115" s="66"/>
       <c r="E115" s="40" t="str">
         <f>overview!C113</f>
         <v>5.2.6</v>
@@ -7642,8 +6505,8 @@
       </c>
     </row>
     <row r="116" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C116" s="72"/>
-      <c r="D116" s="69"/>
+      <c r="C116" s="60"/>
+      <c r="D116" s="66"/>
       <c r="E116" s="40" t="str">
         <f>overview!C114</f>
         <v>5.2.7</v>
@@ -7654,8 +6517,8 @@
       </c>
     </row>
     <row r="117" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C117" s="72"/>
-      <c r="D117" s="69" t="str">
+      <c r="C117" s="60"/>
+      <c r="D117" s="66" t="str">
         <f>overview!B115</f>
         <v>5.3 проверить наличие, расположение, графический интерфейс формы "пополнить мобильный телефон"</v>
       </c>
@@ -7669,8 +6532,8 @@
       </c>
     </row>
     <row r="118" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C118" s="72"/>
-      <c r="D118" s="69"/>
+      <c r="C118" s="60"/>
+      <c r="D118" s="66"/>
       <c r="E118" s="40" t="str">
         <f>overview!C116</f>
         <v>5.3.2</v>
@@ -7681,8 +6544,8 @@
       </c>
     </row>
     <row r="119" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C119" s="72"/>
-      <c r="D119" s="69"/>
+      <c r="C119" s="60"/>
+      <c r="D119" s="66"/>
       <c r="E119" s="40" t="str">
         <f>overview!C117</f>
         <v>5.3.3</v>
@@ -7693,8 +6556,8 @@
       </c>
     </row>
     <row r="120" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C120" s="72"/>
-      <c r="D120" s="69"/>
+      <c r="C120" s="60"/>
+      <c r="D120" s="66"/>
       <c r="E120" s="40" t="str">
         <f>overview!C118</f>
         <v>5.3.4</v>
@@ -7705,8 +6568,8 @@
       </c>
     </row>
     <row r="121" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C121" s="72"/>
-      <c r="D121" s="69"/>
+      <c r="C121" s="60"/>
+      <c r="D121" s="66"/>
       <c r="E121" s="40" t="str">
         <f>overview!C119</f>
         <v>5.3.5</v>
@@ -7717,8 +6580,8 @@
       </c>
     </row>
     <row r="122" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C122" s="72"/>
-      <c r="D122" s="69"/>
+      <c r="C122" s="60"/>
+      <c r="D122" s="66"/>
       <c r="E122" s="40" t="str">
         <f>overview!C120</f>
         <v>5.3.6</v>
@@ -7729,8 +6592,8 @@
       </c>
     </row>
     <row r="123" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C123" s="72"/>
-      <c r="D123" s="69"/>
+      <c r="C123" s="60"/>
+      <c r="D123" s="66"/>
       <c r="E123" s="40" t="str">
         <f>overview!C121</f>
         <v>5.3.7</v>
@@ -7741,8 +6604,8 @@
       </c>
     </row>
     <row r="124" spans="3:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C124" s="73"/>
-      <c r="D124" s="70"/>
+      <c r="C124" s="61"/>
+      <c r="D124" s="67"/>
       <c r="E124" s="51" t="str">
         <f>overview!C122</f>
         <v>5.3.8</v>
@@ -7753,11 +6616,11 @@
       </c>
     </row>
     <row r="125" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C125" s="74" t="str">
+      <c r="C125" s="62" t="str">
         <f>FRD!A14</f>
         <v>6. Раздел "переводы"</v>
       </c>
-      <c r="D125" s="68" t="str">
+      <c r="D125" s="65" t="str">
         <f>overview!B123</f>
         <v>6.1 проверить наличие, расположение, графический интерфейс раздела "переводы"</v>
       </c>
@@ -7771,8 +6634,8 @@
       </c>
     </row>
     <row r="126" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C126" s="75"/>
-      <c r="D126" s="69"/>
+      <c r="C126" s="63"/>
+      <c r="D126" s="66"/>
       <c r="E126" s="40" t="str">
         <f>overview!C124</f>
         <v>6.1.2</v>
@@ -7783,8 +6646,8 @@
       </c>
     </row>
     <row r="127" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C127" s="75"/>
-      <c r="D127" s="69"/>
+      <c r="C127" s="63"/>
+      <c r="D127" s="66"/>
       <c r="E127" s="40" t="str">
         <f>overview!C125</f>
         <v>6.1.3</v>
@@ -7795,8 +6658,8 @@
       </c>
     </row>
     <row r="128" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C128" s="75"/>
-      <c r="D128" s="69"/>
+      <c r="C128" s="63"/>
+      <c r="D128" s="66"/>
       <c r="E128" s="40" t="str">
         <f>overview!C126</f>
         <v>6.1.4</v>
@@ -7807,8 +6670,8 @@
       </c>
     </row>
     <row r="129" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C129" s="75"/>
-      <c r="D129" s="69"/>
+      <c r="C129" s="63"/>
+      <c r="D129" s="66"/>
       <c r="E129" s="40" t="str">
         <f>overview!C127</f>
         <v>6.1.5</v>
@@ -7819,8 +6682,8 @@
       </c>
     </row>
     <row r="130" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C130" s="75"/>
-      <c r="D130" s="69"/>
+      <c r="C130" s="63"/>
+      <c r="D130" s="66"/>
       <c r="E130" s="40" t="str">
         <f>overview!C128</f>
         <v>6.1.6</v>
@@ -7831,8 +6694,8 @@
       </c>
     </row>
     <row r="131" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C131" s="75"/>
-      <c r="D131" s="69"/>
+      <c r="C131" s="63"/>
+      <c r="D131" s="66"/>
       <c r="E131" s="40" t="str">
         <f>overview!C129</f>
         <v>6.1.7</v>
@@ -7843,8 +6706,8 @@
       </c>
     </row>
     <row r="132" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C132" s="75"/>
-      <c r="D132" s="69"/>
+      <c r="C132" s="63"/>
+      <c r="D132" s="66"/>
       <c r="E132" s="40" t="str">
         <f>overview!C130</f>
         <v>6.1.8</v>
@@ -7855,8 +6718,8 @@
       </c>
     </row>
     <row r="133" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C133" s="75"/>
-      <c r="D133" s="69"/>
+      <c r="C133" s="63"/>
+      <c r="D133" s="66"/>
       <c r="E133" s="40" t="str">
         <f>overview!C131</f>
         <v>6.1.9</v>
@@ -7867,8 +6730,8 @@
       </c>
     </row>
     <row r="134" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C134" s="75"/>
-      <c r="D134" s="69"/>
+      <c r="C134" s="63"/>
+      <c r="D134" s="66"/>
       <c r="E134" s="40" t="str">
         <f>overview!C132</f>
         <v>6.1.10</v>
@@ -7879,8 +6742,8 @@
       </c>
     </row>
     <row r="135" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C135" s="75"/>
-      <c r="D135" s="69"/>
+      <c r="C135" s="63"/>
+      <c r="D135" s="66"/>
       <c r="E135" s="40" t="str">
         <f>overview!C133</f>
         <v>6.1.11</v>
@@ -7891,8 +6754,8 @@
       </c>
     </row>
     <row r="136" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C136" s="75"/>
-      <c r="D136" s="69" t="str">
+      <c r="C136" s="63"/>
+      <c r="D136" s="66" t="str">
         <f>overview!B134</f>
         <v>6.2 Проверить ввода данных раздела "переводы"</v>
       </c>
@@ -7906,8 +6769,8 @@
       </c>
     </row>
     <row r="137" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C137" s="75"/>
-      <c r="D137" s="69"/>
+      <c r="C137" s="63"/>
+      <c r="D137" s="66"/>
       <c r="E137" s="40" t="str">
         <f>overview!C135</f>
         <v>6.2.2</v>
@@ -7918,8 +6781,8 @@
       </c>
     </row>
     <row r="138" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C138" s="75"/>
-      <c r="D138" s="69"/>
+      <c r="C138" s="63"/>
+      <c r="D138" s="66"/>
       <c r="E138" s="40" t="str">
         <f>overview!C136</f>
         <v>6.2.3</v>
@@ -7930,8 +6793,8 @@
       </c>
     </row>
     <row r="139" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C139" s="75"/>
-      <c r="D139" s="69"/>
+      <c r="C139" s="63"/>
+      <c r="D139" s="66"/>
       <c r="E139" s="40" t="str">
         <f>overview!C137</f>
         <v>6.2.4</v>
@@ -7942,8 +6805,8 @@
       </c>
     </row>
     <row r="140" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C140" s="75"/>
-      <c r="D140" s="69"/>
+      <c r="C140" s="63"/>
+      <c r="D140" s="66"/>
       <c r="E140" s="40" t="str">
         <f>overview!C138</f>
         <v>6.2.5</v>
@@ -7954,8 +6817,8 @@
       </c>
     </row>
     <row r="141" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C141" s="75"/>
-      <c r="D141" s="69"/>
+      <c r="C141" s="63"/>
+      <c r="D141" s="66"/>
       <c r="E141" s="40" t="str">
         <f>overview!C139</f>
         <v>6.2.6</v>
@@ -7966,8 +6829,8 @@
       </c>
     </row>
     <row r="142" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C142" s="75"/>
-      <c r="D142" s="69"/>
+      <c r="C142" s="63"/>
+      <c r="D142" s="66"/>
       <c r="E142" s="40" t="str">
         <f>overview!C140</f>
         <v>6.2.7</v>
@@ -7978,8 +6841,8 @@
       </c>
     </row>
     <row r="143" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C143" s="75"/>
-      <c r="D143" s="69"/>
+      <c r="C143" s="63"/>
+      <c r="D143" s="66"/>
       <c r="E143" s="40" t="str">
         <f>overview!C141</f>
         <v>6.2.8</v>
@@ -7990,8 +6853,8 @@
       </c>
     </row>
     <row r="144" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C144" s="75"/>
-      <c r="D144" s="69"/>
+      <c r="C144" s="63"/>
+      <c r="D144" s="66"/>
       <c r="E144" s="40" t="str">
         <f>overview!C142</f>
         <v>6.2.9</v>
@@ -8002,8 +6865,8 @@
       </c>
     </row>
     <row r="145" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C145" s="75"/>
-      <c r="D145" s="69" t="str">
+      <c r="C145" s="63"/>
+      <c r="D145" s="66" t="str">
         <f>overview!B143</f>
         <v>6.3 Проверить кликабельность, соответствие и коректность формы раздела "переводы"</v>
       </c>
@@ -8017,8 +6880,8 @@
       </c>
     </row>
     <row r="146" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C146" s="75"/>
-      <c r="D146" s="69"/>
+      <c r="C146" s="63"/>
+      <c r="D146" s="66"/>
       <c r="E146" s="40" t="str">
         <f>overview!C144</f>
         <v>6.3.2</v>
@@ -8029,8 +6892,8 @@
       </c>
     </row>
     <row r="147" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C147" s="75"/>
-      <c r="D147" s="69"/>
+      <c r="C147" s="63"/>
+      <c r="D147" s="66"/>
       <c r="E147" s="40" t="str">
         <f>overview!C145</f>
         <v>6.3.3</v>
@@ -8041,8 +6904,8 @@
       </c>
     </row>
     <row r="148" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C148" s="75"/>
-      <c r="D148" s="69"/>
+      <c r="C148" s="63"/>
+      <c r="D148" s="66"/>
       <c r="E148" s="40" t="str">
         <f>overview!C146</f>
         <v>6.3.4</v>
@@ -8053,8 +6916,8 @@
       </c>
     </row>
     <row r="149" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C149" s="75"/>
-      <c r="D149" s="69"/>
+      <c r="C149" s="63"/>
+      <c r="D149" s="66"/>
       <c r="E149" s="40" t="str">
         <f>overview!C147</f>
         <v>6.3.5</v>
@@ -8065,8 +6928,8 @@
       </c>
     </row>
     <row r="150" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C150" s="75"/>
-      <c r="D150" s="69"/>
+      <c r="C150" s="63"/>
+      <c r="D150" s="66"/>
       <c r="E150" s="40" t="str">
         <f>overview!C148</f>
         <v>6.3.6</v>
@@ -8077,8 +6940,8 @@
       </c>
     </row>
     <row r="151" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C151" s="75"/>
-      <c r="D151" s="69"/>
+      <c r="C151" s="63"/>
+      <c r="D151" s="66"/>
       <c r="E151" s="40" t="str">
         <f>overview!C149</f>
         <v>6.3.7</v>
@@ -8089,8 +6952,8 @@
       </c>
     </row>
     <row r="152" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C152" s="76"/>
-      <c r="D152" s="70"/>
+      <c r="C152" s="64"/>
+      <c r="D152" s="67"/>
       <c r="E152" s="51" t="str">
         <f>overview!C150</f>
         <v>6.3.8</v>
@@ -8101,11 +6964,11 @@
       </c>
     </row>
     <row r="153" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C153" s="74" t="str">
+      <c r="C153" s="62" t="str">
         <f>FRD!A16</f>
         <v>7. Раздел "каталог услуг"</v>
       </c>
-      <c r="D153" s="68" t="str">
+      <c r="D153" s="65" t="str">
         <f>overview!B151</f>
         <v>7.1 проверить наличие, расположение, графический интерфейс раздела "каталог услуг"</v>
       </c>
@@ -8119,8 +6982,8 @@
       </c>
     </row>
     <row r="154" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C154" s="75"/>
-      <c r="D154" s="69"/>
+      <c r="C154" s="63"/>
+      <c r="D154" s="66"/>
       <c r="E154" s="40" t="str">
         <f>overview!C152</f>
         <v>7.1.2</v>
@@ -8131,8 +6994,8 @@
       </c>
     </row>
     <row r="155" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C155" s="75"/>
-      <c r="D155" s="69"/>
+      <c r="C155" s="63"/>
+      <c r="D155" s="66"/>
       <c r="E155" s="40" t="str">
         <f>overview!C153</f>
         <v>7.1.3</v>
@@ -8143,8 +7006,8 @@
       </c>
     </row>
     <row r="156" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C156" s="75"/>
-      <c r="D156" s="69"/>
+      <c r="C156" s="63"/>
+      <c r="D156" s="66"/>
       <c r="E156" s="40" t="str">
         <f>overview!C154</f>
         <v>7.1.4</v>
@@ -8155,8 +7018,8 @@
       </c>
     </row>
     <row r="157" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C157" s="75"/>
-      <c r="D157" s="69"/>
+      <c r="C157" s="63"/>
+      <c r="D157" s="66"/>
       <c r="E157" s="40" t="str">
         <f>overview!C155</f>
         <v>7.1.5</v>
@@ -8167,8 +7030,8 @@
       </c>
     </row>
     <row r="158" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C158" s="75"/>
-      <c r="D158" s="69"/>
+      <c r="C158" s="63"/>
+      <c r="D158" s="66"/>
       <c r="E158" s="40" t="str">
         <f>overview!C156</f>
         <v>7.1.6</v>
@@ -8179,8 +7042,8 @@
       </c>
     </row>
     <row r="159" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C159" s="75"/>
-      <c r="D159" s="69"/>
+      <c r="C159" s="63"/>
+      <c r="D159" s="66"/>
       <c r="E159" s="40" t="str">
         <f>overview!C157</f>
         <v>7.1.7</v>
@@ -8191,8 +7054,8 @@
       </c>
     </row>
     <row r="160" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C160" s="75"/>
-      <c r="D160" s="69"/>
+      <c r="C160" s="63"/>
+      <c r="D160" s="66"/>
       <c r="E160" s="40" t="str">
         <f>overview!C158</f>
         <v>7.1.8</v>
@@ -8203,8 +7066,8 @@
       </c>
     </row>
     <row r="161" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C161" s="75"/>
-      <c r="D161" s="69"/>
+      <c r="C161" s="63"/>
+      <c r="D161" s="66"/>
       <c r="E161" s="40" t="str">
         <f>overview!C159</f>
         <v>7.1.9</v>
@@ -8215,8 +7078,8 @@
       </c>
     </row>
     <row r="162" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C162" s="75"/>
-      <c r="D162" s="69"/>
+      <c r="C162" s="63"/>
+      <c r="D162" s="66"/>
       <c r="E162" s="40" t="str">
         <f>overview!C160</f>
         <v>7.1.10</v>
@@ -8227,8 +7090,8 @@
       </c>
     </row>
     <row r="163" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C163" s="75"/>
-      <c r="D163" s="69"/>
+      <c r="C163" s="63"/>
+      <c r="D163" s="66"/>
       <c r="E163" s="40" t="str">
         <f>overview!C161</f>
         <v>7.1.11</v>
@@ -8239,8 +7102,8 @@
       </c>
     </row>
     <row r="164" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C164" s="75"/>
-      <c r="D164" s="69" t="str">
+      <c r="C164" s="63"/>
+      <c r="D164" s="66" t="str">
         <f>overview!B162</f>
         <v>7.2 Проверить кликабельность, соответствие и коректность формы раздела "каталог услуг"</v>
       </c>
@@ -8254,8 +7117,8 @@
       </c>
     </row>
     <row r="165" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C165" s="75"/>
-      <c r="D165" s="69"/>
+      <c r="C165" s="63"/>
+      <c r="D165" s="66"/>
       <c r="E165" s="40" t="str">
         <f>overview!C163</f>
         <v>7.2.2</v>
@@ -8266,8 +7129,8 @@
       </c>
     </row>
     <row r="166" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C166" s="75"/>
-      <c r="D166" s="69"/>
+      <c r="C166" s="63"/>
+      <c r="D166" s="66"/>
       <c r="E166" s="40" t="str">
         <f>overview!C164</f>
         <v>7.2.3</v>
@@ -8278,8 +7141,8 @@
       </c>
     </row>
     <row r="167" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C167" s="75"/>
-      <c r="D167" s="69"/>
+      <c r="C167" s="63"/>
+      <c r="D167" s="66"/>
       <c r="E167" s="40" t="str">
         <f>overview!C165</f>
         <v>7.2.4</v>
@@ -8290,8 +7153,8 @@
       </c>
     </row>
     <row r="168" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C168" s="75"/>
-      <c r="D168" s="69"/>
+      <c r="C168" s="63"/>
+      <c r="D168" s="66"/>
       <c r="E168" s="40" t="str">
         <f>overview!C166</f>
         <v>7.2.5</v>
@@ -8302,8 +7165,8 @@
       </c>
     </row>
     <row r="169" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C169" s="75"/>
-      <c r="D169" s="69"/>
+      <c r="C169" s="63"/>
+      <c r="D169" s="66"/>
       <c r="E169" s="40" t="str">
         <f>overview!C167</f>
         <v>7.2.6</v>
@@ -8314,8 +7177,8 @@
       </c>
     </row>
     <row r="170" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C170" s="75"/>
-      <c r="D170" s="69"/>
+      <c r="C170" s="63"/>
+      <c r="D170" s="66"/>
       <c r="E170" s="40" t="str">
         <f>overview!C168</f>
         <v>7.2.7</v>
@@ -8326,8 +7189,8 @@
       </c>
     </row>
     <row r="171" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C171" s="76"/>
-      <c r="D171" s="70"/>
+      <c r="C171" s="64"/>
+      <c r="D171" s="67"/>
       <c r="E171" s="51" t="str">
         <f>overview!C169</f>
         <v>7.2.8</v>
@@ -8338,11 +7201,11 @@
       </c>
     </row>
     <row r="172" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C172" s="71" t="str">
+      <c r="C172" s="59" t="str">
         <f>FRD!A18</f>
         <v>8. Раздел "оплата по реквизитам"</v>
       </c>
-      <c r="D172" s="68" t="str">
+      <c r="D172" s="65" t="str">
         <f>overview!B170</f>
         <v>8.1 проверить наличие, расположение, графический интерфейс раздела "оплата по реквизитам"</v>
       </c>
@@ -8356,8 +7219,8 @@
       </c>
     </row>
     <row r="173" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C173" s="72"/>
-      <c r="D173" s="69"/>
+      <c r="C173" s="60"/>
+      <c r="D173" s="66"/>
       <c r="E173" s="40" t="str">
         <f>overview!C171</f>
         <v>8.1.2</v>
@@ -8368,8 +7231,8 @@
       </c>
     </row>
     <row r="174" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C174" s="72"/>
-      <c r="D174" s="69"/>
+      <c r="C174" s="60"/>
+      <c r="D174" s="66"/>
       <c r="E174" s="40" t="str">
         <f>overview!C172</f>
         <v>8.1.3</v>
@@ -8380,8 +7243,8 @@
       </c>
     </row>
     <row r="175" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C175" s="72"/>
-      <c r="D175" s="69"/>
+      <c r="C175" s="60"/>
+      <c r="D175" s="66"/>
       <c r="E175" s="40" t="str">
         <f>overview!C173</f>
         <v>8.1.4</v>
@@ -8392,8 +7255,8 @@
       </c>
     </row>
     <row r="176" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C176" s="72"/>
-      <c r="D176" s="69"/>
+      <c r="C176" s="60"/>
+      <c r="D176" s="66"/>
       <c r="E176" s="40" t="str">
         <f>overview!C174</f>
         <v>8.1.5</v>
@@ -8404,8 +7267,8 @@
       </c>
     </row>
     <row r="177" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C177" s="72"/>
-      <c r="D177" s="69"/>
+      <c r="C177" s="60"/>
+      <c r="D177" s="66"/>
       <c r="E177" s="40" t="str">
         <f>overview!C175</f>
         <v>8.1.6</v>
@@ -8416,8 +7279,8 @@
       </c>
     </row>
     <row r="178" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C178" s="72"/>
-      <c r="D178" s="69"/>
+      <c r="C178" s="60"/>
+      <c r="D178" s="66"/>
       <c r="E178" s="40" t="str">
         <f>overview!C176</f>
         <v>8.1.7</v>
@@ -8428,8 +7291,8 @@
       </c>
     </row>
     <row r="179" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C179" s="72"/>
-      <c r="D179" s="69"/>
+      <c r="C179" s="60"/>
+      <c r="D179" s="66"/>
       <c r="E179" s="40" t="str">
         <f>overview!C177</f>
         <v>8.1.8</v>
@@ -8440,8 +7303,8 @@
       </c>
     </row>
     <row r="180" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C180" s="72"/>
-      <c r="D180" s="69"/>
+      <c r="C180" s="60"/>
+      <c r="D180" s="66"/>
       <c r="E180" s="40" t="str">
         <f>overview!C178</f>
         <v>8.1.9</v>
@@ -8452,8 +7315,8 @@
       </c>
     </row>
     <row r="181" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C181" s="72"/>
-      <c r="D181" s="69"/>
+      <c r="C181" s="60"/>
+      <c r="D181" s="66"/>
       <c r="E181" s="40" t="str">
         <f>overview!C179</f>
         <v>8.1.10</v>
@@ -8464,8 +7327,8 @@
       </c>
     </row>
     <row r="182" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C182" s="72"/>
-      <c r="D182" s="69"/>
+      <c r="C182" s="60"/>
+      <c r="D182" s="66"/>
       <c r="E182" s="40" t="str">
         <f>overview!C180</f>
         <v>8.1.11</v>
@@ -8476,8 +7339,8 @@
       </c>
     </row>
     <row r="183" spans="3:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C183" s="72"/>
-      <c r="D183" s="69" t="str">
+      <c r="C183" s="60"/>
+      <c r="D183" s="66" t="str">
         <f>overview!B181</f>
         <v>8.2 Проверить ввода данных раздела "оплата по реквизитам"</v>
       </c>
@@ -8491,8 +7354,8 @@
       </c>
     </row>
     <row r="184" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C184" s="72"/>
-      <c r="D184" s="69"/>
+      <c r="C184" s="60"/>
+      <c r="D184" s="66"/>
       <c r="E184" s="40" t="str">
         <f>overview!C182</f>
         <v>8.2.2</v>
@@ -8503,8 +7366,8 @@
       </c>
     </row>
     <row r="185" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C185" s="72"/>
-      <c r="D185" s="69"/>
+      <c r="C185" s="60"/>
+      <c r="D185" s="66"/>
       <c r="E185" s="40" t="str">
         <f>overview!C183</f>
         <v>8.2.3</v>
@@ -8515,8 +7378,8 @@
       </c>
     </row>
     <row r="186" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C186" s="72"/>
-      <c r="D186" s="69"/>
+      <c r="C186" s="60"/>
+      <c r="D186" s="66"/>
       <c r="E186" s="40" t="str">
         <f>overview!C184</f>
         <v>8.2.4</v>
@@ -8527,8 +7390,8 @@
       </c>
     </row>
     <row r="187" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C187" s="72"/>
-      <c r="D187" s="69"/>
+      <c r="C187" s="60"/>
+      <c r="D187" s="66"/>
       <c r="E187" s="40" t="str">
         <f>overview!C185</f>
         <v>8.2.5</v>
@@ -8539,8 +7402,8 @@
       </c>
     </row>
     <row r="188" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C188" s="72"/>
-      <c r="D188" s="69"/>
+      <c r="C188" s="60"/>
+      <c r="D188" s="66"/>
       <c r="E188" s="40" t="str">
         <f>overview!C186</f>
         <v>8.2.6</v>
@@ -8551,8 +7414,8 @@
       </c>
     </row>
     <row r="189" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C189" s="72"/>
-      <c r="D189" s="69"/>
+      <c r="C189" s="60"/>
+      <c r="D189" s="66"/>
       <c r="E189" s="40" t="str">
         <f>overview!C187</f>
         <v>8.2.7</v>
@@ -8563,8 +7426,8 @@
       </c>
     </row>
     <row r="190" spans="3:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C190" s="72"/>
-      <c r="D190" s="69"/>
+      <c r="C190" s="60"/>
+      <c r="D190" s="66"/>
       <c r="E190" s="40" t="str">
         <f>overview!C188</f>
         <v>8.2.8</v>
@@ -8575,8 +7438,8 @@
       </c>
     </row>
     <row r="191" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C191" s="72"/>
-      <c r="D191" s="69"/>
+      <c r="C191" s="60"/>
+      <c r="D191" s="66"/>
       <c r="E191" s="40" t="str">
         <f>overview!C189</f>
         <v>8.2.9</v>
@@ -8587,8 +7450,8 @@
       </c>
     </row>
     <row r="192" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C192" s="72"/>
-      <c r="D192" s="69" t="str">
+      <c r="C192" s="60"/>
+      <c r="D192" s="66" t="str">
         <f>overview!B190</f>
         <v>8.3 Проверить кликабельность, соответствие и коректность формы раздела "оплата по реквизитам"</v>
       </c>
@@ -8602,8 +7465,8 @@
       </c>
     </row>
     <row r="193" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C193" s="72"/>
-      <c r="D193" s="69"/>
+      <c r="C193" s="60"/>
+      <c r="D193" s="66"/>
       <c r="E193" s="40" t="str">
         <f>overview!C191</f>
         <v>8.3.2</v>
@@ -8614,8 +7477,8 @@
       </c>
     </row>
     <row r="194" spans="3:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C194" s="72"/>
-      <c r="D194" s="69"/>
+      <c r="C194" s="60"/>
+      <c r="D194" s="66"/>
       <c r="E194" s="40" t="str">
         <f>overview!C192</f>
         <v>8.3.3</v>
@@ -8626,8 +7489,8 @@
       </c>
     </row>
     <row r="195" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C195" s="72"/>
-      <c r="D195" s="69"/>
+      <c r="C195" s="60"/>
+      <c r="D195" s="66"/>
       <c r="E195" s="40" t="str">
         <f>overview!C193</f>
         <v>8.3.4</v>
@@ -8638,8 +7501,8 @@
       </c>
     </row>
     <row r="196" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C196" s="72"/>
-      <c r="D196" s="69"/>
+      <c r="C196" s="60"/>
+      <c r="D196" s="66"/>
       <c r="E196" s="40" t="str">
         <f>overview!C194</f>
         <v>8.3.5</v>
@@ -8650,8 +7513,8 @@
       </c>
     </row>
     <row r="197" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C197" s="72"/>
-      <c r="D197" s="69"/>
+      <c r="C197" s="60"/>
+      <c r="D197" s="66"/>
       <c r="E197" s="40" t="str">
         <f>overview!C195</f>
         <v>8.3.6</v>
@@ -8662,8 +7525,8 @@
       </c>
     </row>
     <row r="198" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C198" s="72"/>
-      <c r="D198" s="69"/>
+      <c r="C198" s="60"/>
+      <c r="D198" s="66"/>
       <c r="E198" s="40" t="str">
         <f>overview!C196</f>
         <v>8.3.7</v>
@@ -8674,8 +7537,8 @@
       </c>
     </row>
     <row r="199" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C199" s="73"/>
-      <c r="D199" s="70"/>
+      <c r="C199" s="61"/>
+      <c r="D199" s="67"/>
       <c r="E199" s="51" t="str">
         <f>overview!C197</f>
         <v>8.3.8</v>
@@ -8686,11 +7549,11 @@
       </c>
     </row>
     <row r="200" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C200" s="71" t="str">
+      <c r="C200" s="59" t="str">
         <f>FRD!A20</f>
         <v>9. Нижний колонтитул</v>
       </c>
-      <c r="D200" s="68" t="str">
+      <c r="D200" s="65" t="str">
         <f>overview!B198</f>
         <v>9.1 проверить наличие, расположение, графический интерфейс раздела "нижний колонтитул"</v>
       </c>
@@ -8704,8 +7567,8 @@
       </c>
     </row>
     <row r="201" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C201" s="72"/>
-      <c r="D201" s="69"/>
+      <c r="C201" s="60"/>
+      <c r="D201" s="66"/>
       <c r="E201" s="40" t="str">
         <f>overview!C199</f>
         <v>9.1.2</v>
@@ -8716,8 +7579,8 @@
       </c>
     </row>
     <row r="202" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C202" s="72"/>
-      <c r="D202" s="69"/>
+      <c r="C202" s="60"/>
+      <c r="D202" s="66"/>
       <c r="E202" s="40" t="str">
         <f>overview!C200</f>
         <v>9.1.3</v>
@@ -8728,8 +7591,8 @@
       </c>
     </row>
     <row r="203" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C203" s="72"/>
-      <c r="D203" s="69"/>
+      <c r="C203" s="60"/>
+      <c r="D203" s="66"/>
       <c r="E203" s="40" t="str">
         <f>overview!C201</f>
         <v>9.1.4</v>
@@ -8740,8 +7603,8 @@
       </c>
     </row>
     <row r="204" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C204" s="72"/>
-      <c r="D204" s="69"/>
+      <c r="C204" s="60"/>
+      <c r="D204" s="66"/>
       <c r="E204" s="40" t="str">
         <f>overview!C202</f>
         <v>9.1.5</v>
@@ -8752,8 +7615,8 @@
       </c>
     </row>
     <row r="205" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C205" s="72"/>
-      <c r="D205" s="69"/>
+      <c r="C205" s="60"/>
+      <c r="D205" s="66"/>
       <c r="E205" s="40" t="str">
         <f>overview!C203</f>
         <v>9.1.6</v>
@@ -8764,8 +7627,8 @@
       </c>
     </row>
     <row r="206" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C206" s="72"/>
-      <c r="D206" s="69"/>
+      <c r="C206" s="60"/>
+      <c r="D206" s="66"/>
       <c r="E206" s="40" t="str">
         <f>overview!C204</f>
         <v>9.1.7</v>
@@ -8776,8 +7639,8 @@
       </c>
     </row>
     <row r="207" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C207" s="72"/>
-      <c r="D207" s="69"/>
+      <c r="C207" s="60"/>
+      <c r="D207" s="66"/>
       <c r="E207" s="40" t="str">
         <f>overview!C205</f>
         <v>9.1.8</v>
@@ -8788,8 +7651,8 @@
       </c>
     </row>
     <row r="208" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C208" s="72"/>
-      <c r="D208" s="69"/>
+      <c r="C208" s="60"/>
+      <c r="D208" s="66"/>
       <c r="E208" s="40" t="str">
         <f>overview!C206</f>
         <v>9.1.9</v>
@@ -8800,8 +7663,8 @@
       </c>
     </row>
     <row r="209" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C209" s="72"/>
-      <c r="D209" s="69"/>
+      <c r="C209" s="60"/>
+      <c r="D209" s="66"/>
       <c r="E209" s="40" t="str">
         <f>overview!C207</f>
         <v>9.1.10</v>
@@ -8812,8 +7675,8 @@
       </c>
     </row>
     <row r="210" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C210" s="72"/>
-      <c r="D210" s="69"/>
+      <c r="C210" s="60"/>
+      <c r="D210" s="66"/>
       <c r="E210" s="40" t="str">
         <f>overview!C208</f>
         <v>9.1.11</v>
@@ -8824,8 +7687,8 @@
       </c>
     </row>
     <row r="211" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C211" s="72"/>
-      <c r="D211" s="69" t="str">
+      <c r="C211" s="60"/>
+      <c r="D211" s="66" t="str">
         <f>overview!B209</f>
         <v>9.2 Проверить кликабельность, соответствие и коректность формы раздела "нижний колонтитул"</v>
       </c>
@@ -8839,8 +7702,8 @@
       </c>
     </row>
     <row r="212" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C212" s="72"/>
-      <c r="D212" s="69"/>
+      <c r="C212" s="60"/>
+      <c r="D212" s="66"/>
       <c r="E212" s="40" t="str">
         <f>overview!C210</f>
         <v>9.2.2</v>
@@ -8851,8 +7714,8 @@
       </c>
     </row>
     <row r="213" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C213" s="72"/>
-      <c r="D213" s="69"/>
+      <c r="C213" s="60"/>
+      <c r="D213" s="66"/>
       <c r="E213" s="40" t="str">
         <f>overview!C211</f>
         <v>9.2.3</v>
@@ -8863,8 +7726,8 @@
       </c>
     </row>
     <row r="214" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C214" s="72"/>
-      <c r="D214" s="69"/>
+      <c r="C214" s="60"/>
+      <c r="D214" s="66"/>
       <c r="E214" s="40" t="str">
         <f>overview!C212</f>
         <v>9.2.4</v>
@@ -8875,8 +7738,8 @@
       </c>
     </row>
     <row r="215" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C215" s="72"/>
-      <c r="D215" s="69"/>
+      <c r="C215" s="60"/>
+      <c r="D215" s="66"/>
       <c r="E215" s="40" t="str">
         <f>overview!C213</f>
         <v>9.2.5</v>
@@ -8887,8 +7750,8 @@
       </c>
     </row>
     <row r="216" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C216" s="72"/>
-      <c r="D216" s="69"/>
+      <c r="C216" s="60"/>
+      <c r="D216" s="66"/>
       <c r="E216" s="40" t="str">
         <f>overview!C214</f>
         <v>9.2.6</v>
@@ -8899,8 +7762,8 @@
       </c>
     </row>
     <row r="217" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C217" s="72"/>
-      <c r="D217" s="69"/>
+      <c r="C217" s="60"/>
+      <c r="D217" s="66"/>
       <c r="E217" s="40" t="str">
         <f>overview!C215</f>
         <v>9.2.7</v>
@@ -8911,8 +7774,8 @@
       </c>
     </row>
     <row r="218" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C218" s="73"/>
-      <c r="D218" s="70"/>
+      <c r="C218" s="61"/>
+      <c r="D218" s="67"/>
       <c r="E218" s="51" t="str">
         <f>overview!C216</f>
         <v>9.2.8</v>
@@ -8924,37 +7787,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="D4:D10"/>
+    <mergeCell ref="D11:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C4:C19"/>
+    <mergeCell ref="D23:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D47:D77"/>
+    <mergeCell ref="D78:D84"/>
+    <mergeCell ref="C20:C43"/>
+    <mergeCell ref="C44:C84"/>
+    <mergeCell ref="D85:D92"/>
+    <mergeCell ref="D93:D100"/>
+    <mergeCell ref="D101:D109"/>
+    <mergeCell ref="D110:D116"/>
+    <mergeCell ref="D117:D124"/>
+    <mergeCell ref="D125:D135"/>
+    <mergeCell ref="D136:D144"/>
+    <mergeCell ref="D145:D152"/>
+    <mergeCell ref="D153:D163"/>
+    <mergeCell ref="D164:D171"/>
+    <mergeCell ref="D172:D182"/>
+    <mergeCell ref="D183:D191"/>
+    <mergeCell ref="D192:D199"/>
+    <mergeCell ref="D200:D210"/>
+    <mergeCell ref="D211:D218"/>
     <mergeCell ref="C200:C218"/>
     <mergeCell ref="C85:C100"/>
     <mergeCell ref="C101:C124"/>
     <mergeCell ref="C125:C152"/>
     <mergeCell ref="C153:C171"/>
     <mergeCell ref="C172:C199"/>
-    <mergeCell ref="D172:D182"/>
-    <mergeCell ref="D183:D191"/>
-    <mergeCell ref="D192:D199"/>
-    <mergeCell ref="D200:D210"/>
-    <mergeCell ref="D211:D218"/>
-    <mergeCell ref="D125:D135"/>
-    <mergeCell ref="D136:D144"/>
-    <mergeCell ref="D145:D152"/>
-    <mergeCell ref="D153:D163"/>
-    <mergeCell ref="D164:D171"/>
-    <mergeCell ref="D85:D92"/>
-    <mergeCell ref="D93:D100"/>
-    <mergeCell ref="D101:D109"/>
-    <mergeCell ref="D110:D116"/>
-    <mergeCell ref="D117:D124"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D47:D77"/>
-    <mergeCell ref="D78:D84"/>
-    <mergeCell ref="C20:C43"/>
-    <mergeCell ref="C44:C84"/>
-    <mergeCell ref="D4:D10"/>
-    <mergeCell ref="D11:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="C4:C19"/>
-    <mergeCell ref="D23:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8977,10 +7840,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="77" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="81"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="3" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25">
@@ -9087,10 +7950,10 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="77" t="s">
         <v>218</v>
       </c>
-      <c r="C17" s="81"/>
+      <c r="C17" s="77"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="27">
@@ -9421,16 +8284,16 @@
       </c>
     </row>
     <row r="60" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="80" t="s">
+      <c r="B60" s="78" t="s">
         <v>299</v>
       </c>
-      <c r="C60" s="80"/>
+      <c r="C60" s="78"/>
     </row>
     <row r="61" spans="2:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="82" t="s">
+      <c r="B61" s="79" t="s">
         <v>300</v>
       </c>
-      <c r="C61" s="83"/>
+      <c r="C61" s="80"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="31">
@@ -9457,16 +8320,16 @@
       </c>
     </row>
     <row r="66" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="80" t="s">
+      <c r="B66" s="78" t="s">
         <v>362</v>
       </c>
-      <c r="C66" s="80"/>
+      <c r="C66" s="78"/>
     </row>
     <row r="67" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="77" t="s">
+      <c r="B67" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="C67" s="78"/>
+      <c r="C67" s="82"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="31">
@@ -9501,10 +8364,10 @@
       </c>
     </row>
     <row r="72" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="77" t="s">
+      <c r="B72" s="81" t="s">
         <v>368</v>
       </c>
-      <c r="C72" s="78"/>
+      <c r="C72" s="82"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="33">
@@ -9587,10 +8450,10 @@
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="79" t="s">
+      <c r="B84" s="83" t="s">
         <v>417</v>
       </c>
-      <c r="C84" s="79"/>
+      <c r="C84" s="83"/>
     </row>
     <row r="85" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="4">
@@ -9697,16 +8560,16 @@
       </c>
     </row>
     <row r="99" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="80" t="s">
+      <c r="B99" s="78" t="s">
         <v>488</v>
       </c>
-      <c r="C99" s="80"/>
+      <c r="C99" s="78"/>
     </row>
     <row r="100" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="77" t="s">
+      <c r="B100" s="81" t="s">
         <v>489</v>
       </c>
-      <c r="C100" s="78"/>
+      <c r="C100" s="82"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="31">
@@ -9821,10 +8684,10 @@
       </c>
     </row>
     <row r="115" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="77" t="s">
+      <c r="B115" s="81" t="s">
         <v>503</v>
       </c>
-      <c r="C115" s="78"/>
+      <c r="C115" s="82"/>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="33">
@@ -9931,10 +8794,10 @@
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B130" s="79" t="s">
+      <c r="B130" s="83" t="s">
         <v>555</v>
       </c>
-      <c r="C130" s="79"/>
+      <c r="C130" s="83"/>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="4">
@@ -10042,11 +8905,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B66:C66"/>
     <mergeCell ref="B115:C115"/>
     <mergeCell ref="B130:C130"/>
     <mergeCell ref="B67:C67"/>
@@ -10054,6 +8912,11 @@
     <mergeCell ref="B84:C84"/>
     <mergeCell ref="B99:C99"/>
     <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B66:C66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -10064,27 +8927,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="89" t="s">
         <v>588</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="88" t="str">
@@ -10184,26 +9047,26 @@
       <c r="L8" s="57"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="84" t="s">
@@ -10212,12 +9075,12 @@
       <c r="B11" s="85"/>
       <c r="C11" s="85"/>
       <c r="D11" s="86"/>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="66" t="s">
         <v>598</v>
       </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="88" t="str">
@@ -10369,26 +9232,26 @@
       <c r="AD19" s="57"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="89" t="s">
+      <c r="A20" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81" t="s">
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F21" s="81"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
     </row>
     <row r="22" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="84" t="s">
@@ -10502,26 +9365,26 @@
       <c r="L29" s="57"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="81" t="s">
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
     </row>
     <row r="32" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="84" t="s">
@@ -10635,26 +9498,26 @@
       <c r="L39" s="57"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="89" t="s">
+      <c r="A40" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B40" s="89"/>
-      <c r="C40" s="89"/>
-      <c r="D40" s="89"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81" t="s">
+      <c r="B41" s="77"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F41" s="81"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="84" t="s">
@@ -10768,26 +9631,26 @@
       <c r="L49" s="57"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="89" t="s">
+      <c r="A50" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B50" s="89"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="81" t="s">
+      <c r="A51" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B51" s="81"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81" t="s">
+      <c r="B51" s="77"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F51" s="81"/>
-      <c r="G51" s="81"/>
-      <c r="H51" s="81"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="77"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="84" t="s">
@@ -10901,26 +9764,26 @@
       <c r="L59" s="57"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="89" t="s">
+      <c r="A60" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B60" s="89"/>
-      <c r="C60" s="89"/>
-      <c r="D60" s="89"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="87"/>
+      <c r="D60" s="87"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B61" s="81"/>
-      <c r="C61" s="81"/>
-      <c r="D61" s="81"/>
-      <c r="E61" s="81" t="s">
+      <c r="B61" s="77"/>
+      <c r="C61" s="77"/>
+      <c r="D61" s="77"/>
+      <c r="E61" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F61" s="81"/>
-      <c r="G61" s="81"/>
-      <c r="H61" s="81"/>
+      <c r="F61" s="77"/>
+      <c r="G61" s="77"/>
+      <c r="H61" s="77"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="84" t="s">
@@ -11034,26 +9897,26 @@
       <c r="L69" s="57"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="89" t="s">
+      <c r="A70" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B70" s="89"/>
-      <c r="C70" s="89"/>
-      <c r="D70" s="89"/>
+      <c r="B70" s="87"/>
+      <c r="C70" s="87"/>
+      <c r="D70" s="87"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="81" t="s">
+      <c r="A71" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B71" s="81"/>
-      <c r="C71" s="81"/>
-      <c r="D71" s="81"/>
-      <c r="E71" s="81" t="s">
+      <c r="B71" s="77"/>
+      <c r="C71" s="77"/>
+      <c r="D71" s="77"/>
+      <c r="E71" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F71" s="81"/>
-      <c r="G71" s="81"/>
-      <c r="H71" s="81"/>
+      <c r="F71" s="77"/>
+      <c r="G71" s="77"/>
+      <c r="H71" s="77"/>
     </row>
     <row r="72" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="84" t="s">
@@ -11151,26 +10014,26 @@
       <c r="L78" s="57"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="89" t="s">
+      <c r="A79" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B79" s="89"/>
-      <c r="C79" s="89"/>
-      <c r="D79" s="89"/>
+      <c r="B79" s="87"/>
+      <c r="C79" s="87"/>
+      <c r="D79" s="87"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="81" t="s">
+      <c r="A80" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B80" s="81"/>
-      <c r="C80" s="81"/>
-      <c r="D80" s="81"/>
-      <c r="E80" s="81" t="s">
+      <c r="B80" s="77"/>
+      <c r="C80" s="77"/>
+      <c r="D80" s="77"/>
+      <c r="E80" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F80" s="81"/>
-      <c r="G80" s="81"/>
-      <c r="H80" s="81"/>
+      <c r="F80" s="77"/>
+      <c r="G80" s="77"/>
+      <c r="H80" s="77"/>
     </row>
     <row r="81" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="84" t="s">
@@ -11284,26 +10147,26 @@
       <c r="L88" s="57"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="89" t="s">
+      <c r="A89" s="87" t="s">
         <v>590</v>
       </c>
-      <c r="B89" s="89"/>
-      <c r="C89" s="89"/>
-      <c r="D89" s="89"/>
+      <c r="B89" s="87"/>
+      <c r="C89" s="87"/>
+      <c r="D89" s="87"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="81" t="s">
+      <c r="A90" s="77" t="s">
         <v>591</v>
       </c>
-      <c r="B90" s="81"/>
-      <c r="C90" s="81"/>
-      <c r="D90" s="81"/>
-      <c r="E90" s="81" t="s">
+      <c r="B90" s="77"/>
+      <c r="C90" s="77"/>
+      <c r="D90" s="77"/>
+      <c r="E90" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="F90" s="81"/>
-      <c r="G90" s="81"/>
-      <c r="H90" s="81"/>
+      <c r="F90" s="77"/>
+      <c r="G90" s="77"/>
+      <c r="H90" s="77"/>
     </row>
     <row r="91" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="84" t="s">
@@ -11321,76 +10184,18 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="E91:H91"/>
-    <mergeCell ref="A88:L88"/>
-    <mergeCell ref="A84:L84"/>
-    <mergeCell ref="A85:L85"/>
-    <mergeCell ref="A86:L86"/>
-    <mergeCell ref="A87:L87"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="E90:H90"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="E80:H80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="E81:H81"/>
-    <mergeCell ref="A83:L83"/>
-    <mergeCell ref="A74:L74"/>
-    <mergeCell ref="A75:L75"/>
-    <mergeCell ref="A76:L76"/>
-    <mergeCell ref="A77:L77"/>
-    <mergeCell ref="A78:L78"/>
-    <mergeCell ref="A68:L68"/>
-    <mergeCell ref="A69:L69"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="E71:H71"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="E72:H72"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="E62:H62"/>
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="A65:L65"/>
-    <mergeCell ref="A66:L66"/>
-    <mergeCell ref="A67:L67"/>
-    <mergeCell ref="A56:L56"/>
-    <mergeCell ref="A57:L57"/>
-    <mergeCell ref="A58:L58"/>
-    <mergeCell ref="A59:L59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="E61:H61"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="E51:H51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="A54:L54"/>
-    <mergeCell ref="A55:L55"/>
-    <mergeCell ref="A45:L45"/>
-    <mergeCell ref="A46:L46"/>
-    <mergeCell ref="A47:L47"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="A49:L49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="A35:L35"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="A37:L37"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="A18:L18"/>
     <mergeCell ref="S17:AD17"/>
     <mergeCell ref="S19:AD19"/>
@@ -11411,317 +10216,77 @@
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="E22:H22"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="A47:L47"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="A49:L49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="A56:L56"/>
+    <mergeCell ref="A57:L57"/>
+    <mergeCell ref="A58:L58"/>
+    <mergeCell ref="A59:L59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="E61:H61"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="A54:L54"/>
+    <mergeCell ref="A55:L55"/>
+    <mergeCell ref="A68:L68"/>
+    <mergeCell ref="A69:L69"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="E62:H62"/>
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="A66:L66"/>
+    <mergeCell ref="A67:L67"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="E80:H80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="A83:L83"/>
+    <mergeCell ref="A74:L74"/>
+    <mergeCell ref="A75:L75"/>
+    <mergeCell ref="A76:L76"/>
+    <mergeCell ref="A77:L77"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="E91:H91"/>
+    <mergeCell ref="A88:L88"/>
+    <mergeCell ref="A84:L84"/>
+    <mergeCell ref="A85:L85"/>
+    <mergeCell ref="A86:L86"/>
+    <mergeCell ref="A87:L87"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="E90:H90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V377"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A360" workbookViewId="0">
-      <selection activeCell="A378" sqref="A378"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
-        <v>635</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
-        <v>636</v>
-      </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="89" t="s">
-        <v>637</v>
-      </c>
-      <c r="B11" s="89"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="89" t="s">
-        <v>638</v>
-      </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89" t="s">
-        <v>639</v>
-      </c>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="89"/>
-      <c r="N17" s="89"/>
-      <c r="P17" s="89" t="s">
-        <v>640</v>
-      </c>
-      <c r="Q17" s="89"/>
-      <c r="R17" s="89"/>
-      <c r="S17" s="89"/>
-      <c r="T17" s="89"/>
-      <c r="U17" s="89"/>
-      <c r="V17" s="89"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="89" t="s">
-        <v>641</v>
-      </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="89"/>
-      <c r="E51" s="89"/>
-      <c r="F51" s="89"/>
-      <c r="G51" s="89"/>
-      <c r="H51" s="89" t="s">
-        <v>642</v>
-      </c>
-      <c r="I51" s="89"/>
-      <c r="J51" s="89"/>
-      <c r="K51" s="89"/>
-      <c r="L51" s="89"/>
-      <c r="M51" s="89"/>
-      <c r="N51" s="89"/>
-      <c r="O51" s="89" t="s">
-        <v>643</v>
-      </c>
-      <c r="P51" s="89"/>
-      <c r="Q51" s="89"/>
-      <c r="R51" s="89"/>
-      <c r="S51" s="89"/>
-      <c r="T51" s="89"/>
-      <c r="U51" s="89"/>
-    </row>
-    <row r="80" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="90" t="s">
-        <v>647</v>
-      </c>
-      <c r="B80" s="90"/>
-      <c r="C80" s="90"/>
-      <c r="D80" s="90"/>
-      <c r="E80" s="90"/>
-      <c r="F80" s="90"/>
-      <c r="G80" s="90"/>
-    </row>
-    <row r="105" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="90" t="s">
-        <v>646</v>
-      </c>
-      <c r="B105" s="90"/>
-      <c r="C105" s="90"/>
-      <c r="D105" s="90"/>
-      <c r="E105" s="90"/>
-      <c r="F105" s="90"/>
-      <c r="G105" s="90"/>
-    </row>
-    <row r="130" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="90" t="s">
-        <v>645</v>
-      </c>
-      <c r="B130" s="90"/>
-      <c r="C130" s="90"/>
-      <c r="D130" s="90"/>
-      <c r="E130" s="90"/>
-      <c r="F130" s="90"/>
-      <c r="G130" s="90"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="90" t="s">
-        <v>644</v>
-      </c>
-      <c r="B155" s="90"/>
-      <c r="C155" s="90"/>
-      <c r="D155" s="90"/>
-      <c r="E155" s="90"/>
-      <c r="F155" s="90"/>
-      <c r="G155" s="90"/>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="90" t="s">
-        <v>648</v>
-      </c>
-      <c r="B180" s="90"/>
-      <c r="C180" s="90"/>
-      <c r="D180" s="90"/>
-      <c r="E180" s="90"/>
-      <c r="F180" s="90"/>
-      <c r="G180" s="90"/>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A205" s="90" t="s">
-        <v>649</v>
-      </c>
-      <c r="B205" s="90"/>
-      <c r="C205" s="90"/>
-      <c r="D205" s="90"/>
-      <c r="E205" s="90"/>
-      <c r="F205" s="90"/>
-      <c r="G205" s="90"/>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" s="90" t="s">
-        <v>650</v>
-      </c>
-      <c r="B230" s="90"/>
-      <c r="C230" s="90"/>
-      <c r="D230" s="90"/>
-      <c r="E230" s="90"/>
-      <c r="F230" s="90"/>
-      <c r="G230" s="90"/>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249" s="90" t="s">
-        <v>651</v>
-      </c>
-      <c r="B249" s="90"/>
-      <c r="C249" s="90"/>
-      <c r="D249" s="90"/>
-      <c r="E249" s="90"/>
-      <c r="F249" s="90"/>
-      <c r="G249" s="90"/>
-    </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="90" t="s">
-        <v>652</v>
-      </c>
-      <c r="B269" s="90"/>
-      <c r="C269" s="90"/>
-      <c r="D269" s="90"/>
-      <c r="E269" s="90"/>
-      <c r="F269" s="90"/>
-      <c r="G269" s="90"/>
-    </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A289" s="90" t="s">
-        <v>653</v>
-      </c>
-      <c r="B289" s="90"/>
-      <c r="C289" s="90"/>
-      <c r="D289" s="90"/>
-      <c r="E289" s="90"/>
-      <c r="F289" s="90"/>
-      <c r="G289" s="90"/>
-    </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A315" s="90" t="s">
-        <v>654</v>
-      </c>
-      <c r="B315" s="90"/>
-      <c r="C315" s="90"/>
-      <c r="D315" s="90"/>
-      <c r="E315" s="90"/>
-      <c r="F315" s="90"/>
-      <c r="G315" s="90"/>
-    </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A342" s="90" t="s">
-        <v>655</v>
-      </c>
-      <c r="B342" s="90"/>
-      <c r="C342" s="90"/>
-      <c r="D342" s="90"/>
-      <c r="E342" s="90"/>
-      <c r="F342" s="90"/>
-      <c r="G342" s="90"/>
-    </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A369" s="90" t="s">
-        <v>656</v>
-      </c>
-      <c r="B369" s="90"/>
-      <c r="C369" s="90"/>
-      <c r="D369" s="90"/>
-      <c r="E369" s="90"/>
-      <c r="F369" s="90"/>
-      <c r="G369" s="90"/>
-    </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A373" s="90" t="s">
-        <v>657</v>
-      </c>
-      <c r="B373" s="90"/>
-      <c r="C373" s="90"/>
-      <c r="D373" s="90"/>
-      <c r="E373" s="90"/>
-      <c r="F373" s="90"/>
-      <c r="G373" s="90"/>
-    </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A377" s="90" t="s">
-        <v>658</v>
-      </c>
-      <c r="B377" s="90"/>
-      <c r="C377" s="90"/>
-      <c r="D377" s="90"/>
-      <c r="E377" s="90"/>
-      <c r="F377" s="90"/>
-      <c r="G377" s="90"/>
-    </row>
-  </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A373:G373"/>
-    <mergeCell ref="A377:G377"/>
-    <mergeCell ref="A269:G269"/>
-    <mergeCell ref="A289:G289"/>
-    <mergeCell ref="A315:G315"/>
-    <mergeCell ref="A342:G342"/>
-    <mergeCell ref="A369:G369"/>
-    <mergeCell ref="P17:V17"/>
-    <mergeCell ref="A180:G180"/>
-    <mergeCell ref="A205:G205"/>
-    <mergeCell ref="A230:G230"/>
-    <mergeCell ref="A249:G249"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="H17:N17"/>
-    <mergeCell ref="A155:G155"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="H51:N51"/>
-    <mergeCell ref="O51:U51"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A105:G105"/>
-    <mergeCell ref="A130:G130"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>